<commit_message>
adding mapping for number of units
</commit_message>
<xml_diff>
--- a/example_project/res_testing_inputs.xlsx
+++ b/example_project/res_testing_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgoldwas/Documents/GitHub/URBANopt/urbanopt-example-geojson-project/example_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961C110C-48F5-404C-977C-32B13D0CE4A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298273D9-E8C7-F647-A89E-2984CA3D93B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="res_testing_inputs" sheetId="1" r:id="rId1"/>
     <sheet name="Inputs Options" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">res_testing_inputs!$A$1:$W$166</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -207,6 +210,24 @@
   <si>
     <t>URBANopt::Scenario::BaselineMapper</t>
   </si>
+  <si>
+    <t>3/28 test results</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>error message</t>
+  </si>
+  <si>
+    <t>Number of errors out of 165 simulations</t>
+  </si>
+  <si>
+    <t>Expected NumberofBedrooms to be less than or equal to (ConditionedFloorArea-120)/70 [context: /HPXML/Building/BuildingDetails/BuildingSummary/BuildingConstruction]</t>
+  </si>
+  <si>
+    <t>["The number of units (8) must be divisible by the number of floors (3).", "Unsuccessful creation of HPXML file."]</t>
+  </si>
 </sst>
 </file>
 
@@ -348,7 +369,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,6 +567,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -707,7 +734,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -716,6 +743,7 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1071,13 +1099,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U166"/>
+  <dimension ref="A1:X169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K138" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B123" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T176" sqref="T176"/>
+      <selection pane="bottomRight" activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1096,9 +1124,13 @@
     <col min="15" max="15" width="31.33203125" style="7" customWidth="1"/>
     <col min="16" max="16" width="21.33203125" style="7" customWidth="1"/>
     <col min="17" max="17" width="35.83203125" style="7" customWidth="1"/>
+    <col min="19" max="20" width="10.83203125" style="8"/>
+    <col min="21" max="21" width="36.1640625" style="8" customWidth="1"/>
+    <col min="23" max="23" width="15.6640625" customWidth="1"/>
+    <col min="24" max="24" width="86.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1150,17 +1182,23 @@
       <c r="Q1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1218,19 +1256,25 @@
       <c r="Q2" s="7">
         <v>600</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="8">
         <f>A2</f>
         <v>1</v>
       </c>
-      <c r="T2" t="str">
+      <c r="T2" s="8" t="str">
         <f>B2</f>
         <v>Multifamily crawlspace - vented attic - vented Residential - electric resistance and no cooling</v>
       </c>
-      <c r="U2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W2" t="s">
+        <v>59</v>
+      </c>
+      <c r="X2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1289,19 +1333,19 @@
       <c r="Q3" s="7">
         <v>800</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="8">
         <f t="shared" ref="S3:S66" si="6">A3</f>
         <v>2</v>
       </c>
-      <c r="T3" t="str">
+      <c r="T3" s="8" t="str">
         <f t="shared" ref="T3:T66" si="7">B3</f>
         <v>Multifamily crawlspace - unvented attic - vented Residential - electric resistance and central air conditioner</v>
       </c>
-      <c r="U3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U3" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A67" si="8">A3+1</f>
         <v>3</v>
@@ -1360,19 +1404,25 @@
       <c r="Q4" s="7">
         <v>1000</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="8">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="T4" t="str">
+      <c r="T4" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - unconditioned attic - vented Residential - electric resistance and room air conditioner</v>
       </c>
-      <c r="U4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4" t="s">
+        <v>59</v>
+      </c>
+      <c r="X4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="8"/>
         <v>4</v>
@@ -1431,19 +1481,19 @@
       <c r="Q5" s="7">
         <v>1500</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="8">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="T5" t="str">
+      <c r="T5" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - conditioned attic - vented Residential - electric resistance and evaporative cooler</v>
       </c>
-      <c r="U5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U5" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="8"/>
         <v>5</v>
@@ -1502,19 +1552,19 @@
       <c r="Q6" s="7">
         <v>2000</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="8">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="T6" t="str">
+      <c r="T6" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily ambient attic - vented Residential - furnace and no cooling</v>
       </c>
-      <c r="U6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U6" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="8"/>
         <v>6</v>
@@ -1573,19 +1623,19 @@
       <c r="Q7" s="7">
         <v>600</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="8">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="T7" t="str">
+      <c r="T7" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - vented attic - unvented Residential - furnace and central air conditioner</v>
       </c>
-      <c r="U7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U7" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="8"/>
         <v>7</v>
@@ -1644,19 +1694,22 @@
       <c r="Q8" s="7">
         <v>800</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="8">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="T8" t="str">
+      <c r="T8" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - unvented attic - unvented Residential - furnace and room air conditioner</v>
       </c>
-      <c r="U8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="8"/>
         <v>8</v>
@@ -1715,19 +1768,19 @@
       <c r="Q9" s="7">
         <v>1000</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="8">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="T9" t="str">
+      <c r="T9" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - unconditioned attic - unvented Residential - furnace and evaporative cooler</v>
       </c>
-      <c r="U9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U9" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="8"/>
         <v>9</v>
@@ -1786,19 +1839,19 @@
       <c r="Q10" s="7">
         <v>1500</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="8">
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="T10" t="str">
+      <c r="T10" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - conditioned attic - unvented Residential - boiler and no cooling</v>
       </c>
-      <c r="U10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U10" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="8"/>
         <v>10</v>
@@ -1857,19 +1910,19 @@
       <c r="Q11" s="7">
         <v>2000</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="8">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="T11" t="str">
+      <c r="T11" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily ambient attic - unvented Residential - boiler and central air conditioner</v>
       </c>
-      <c r="U11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U11" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="8"/>
         <v>11</v>
@@ -1928,19 +1981,22 @@
       <c r="Q12" s="7">
         <v>600</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="8">
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
-      <c r="T12" t="str">
+      <c r="T12" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - vented attic - conditioned Residential - boiler and room air conditioner</v>
       </c>
-      <c r="U12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="8"/>
         <v>12</v>
@@ -1999,19 +2055,19 @@
       <c r="Q13" s="7">
         <v>800</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="8">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="T13" t="str">
+      <c r="T13" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - unvented attic - conditioned Residential - boiler and evaporative cooler</v>
       </c>
-      <c r="U13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U13" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="8"/>
         <v>13</v>
@@ -2070,19 +2126,22 @@
       <c r="Q14" s="7">
         <v>1000</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="8">
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="T14" t="str">
+      <c r="T14" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - unconditioned attic - conditioned Residential - air-to-air heat pump</v>
       </c>
-      <c r="U14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="8"/>
         <v>14</v>
@@ -2141,19 +2200,19 @@
       <c r="Q15" s="7">
         <v>1500</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="8">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="T15" t="str">
+      <c r="T15" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - conditioned attic - conditioned Residential - mini-split heat pump</v>
       </c>
-      <c r="U15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U15" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="8"/>
         <v>15</v>
@@ -2212,19 +2271,22 @@
       <c r="Q16" s="7">
         <v>2000</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="8">
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="T16" t="str">
+      <c r="T16" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily ambient attic - conditioned Residential - ground-to-air heat pump</v>
       </c>
-      <c r="U16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="8"/>
         <v>16</v>
@@ -2283,19 +2345,19 @@
       <c r="Q17" s="7">
         <v>600</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="8">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="T17" t="str">
+      <c r="T17" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - vented flat roof Residential - electric resistance and no cooling</v>
       </c>
-      <c r="U17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U17" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="8"/>
         <v>17</v>
@@ -2354,19 +2416,22 @@
       <c r="Q18" s="7">
         <v>800</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="8">
         <f t="shared" si="6"/>
         <v>17</v>
       </c>
-      <c r="T18" t="str">
+      <c r="T18" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - unvented flat roof Residential - electric resistance and central air conditioner</v>
       </c>
-      <c r="U18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -2425,19 +2490,19 @@
       <c r="Q19" s="7">
         <v>1000</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="8">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="T19" t="str">
+      <c r="T19" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - unconditioned flat roof Residential - electric resistance and room air conditioner</v>
       </c>
-      <c r="U19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U19" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -2496,19 +2561,22 @@
       <c r="Q20" s="7">
         <v>1500</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="8">
         <f t="shared" si="6"/>
         <v>19</v>
       </c>
-      <c r="T20" t="str">
+      <c r="T20" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - conditioned flat roof Residential - electric resistance and evaporative cooler</v>
       </c>
-      <c r="U20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U20" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -2567,19 +2635,19 @@
       <c r="Q21" s="7">
         <v>2000</v>
       </c>
-      <c r="S21">
+      <c r="S21" s="8">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="T21" t="str">
+      <c r="T21" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily ambient flat roof Residential - furnace and no cooling</v>
       </c>
-      <c r="U21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U21" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -2638,19 +2706,22 @@
       <c r="Q22" s="7">
         <v>600</v>
       </c>
-      <c r="S22">
+      <c r="S22" s="8">
         <f t="shared" si="6"/>
         <v>21</v>
       </c>
-      <c r="T22" t="str">
+      <c r="T22" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - vented attic - vented Residential - furnace and central air conditioner</v>
       </c>
-      <c r="U22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U22" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -2709,19 +2780,19 @@
       <c r="Q23" s="7">
         <v>800</v>
       </c>
-      <c r="S23">
+      <c r="S23" s="8">
         <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="T23" t="str">
+      <c r="T23" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - unvented attic - vented Residential - furnace and room air conditioner</v>
       </c>
-      <c r="U23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U23" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -2780,19 +2851,22 @@
       <c r="Q24" s="7">
         <v>1000</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="8">
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="T24" t="str">
+      <c r="T24" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - unconditioned attic - vented Residential - furnace and evaporative cooler</v>
       </c>
-      <c r="U24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U24" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -2851,19 +2925,19 @@
       <c r="Q25" s="7">
         <v>1500</v>
       </c>
-      <c r="S25">
+      <c r="S25" s="8">
         <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="T25" t="str">
+      <c r="T25" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - conditioned attic - vented Residential - boiler and no cooling</v>
       </c>
-      <c r="U25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U25" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="8"/>
         <v>25</v>
@@ -2922,19 +2996,19 @@
       <c r="Q26" s="7">
         <v>2000</v>
       </c>
-      <c r="S26">
+      <c r="S26" s="8">
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="T26" t="str">
+      <c r="T26" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily ambient attic - vented Residential - boiler and central air conditioner</v>
       </c>
-      <c r="U26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U26" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="8"/>
         <v>26</v>
@@ -2993,19 +3067,19 @@
       <c r="Q27" s="7">
         <v>600</v>
       </c>
-      <c r="S27">
+      <c r="S27" s="8">
         <f t="shared" si="6"/>
         <v>26</v>
       </c>
-      <c r="T27" t="str">
+      <c r="T27" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - vented attic - unvented Residential - boiler and room air conditioner</v>
       </c>
-      <c r="U27" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U27" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="8"/>
         <v>27</v>
@@ -3064,19 +3138,22 @@
       <c r="Q28" s="7">
         <v>800</v>
       </c>
-      <c r="S28">
+      <c r="S28" s="8">
         <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="T28" t="str">
+      <c r="T28" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - unvented attic - unvented Residential - boiler and evaporative cooler</v>
       </c>
-      <c r="U28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U28" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="8"/>
         <v>28</v>
@@ -3135,19 +3212,19 @@
       <c r="Q29" s="7">
         <v>1000</v>
       </c>
-      <c r="S29">
+      <c r="S29" s="8">
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="T29" t="str">
+      <c r="T29" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - unconditioned attic - unvented Residential - air-to-air heat pump</v>
       </c>
-      <c r="U29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U29" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="8"/>
         <v>29</v>
@@ -3206,19 +3283,19 @@
       <c r="Q30" s="7">
         <v>1500</v>
       </c>
-      <c r="S30">
+      <c r="S30" s="8">
         <f t="shared" si="6"/>
         <v>29</v>
       </c>
-      <c r="T30" t="str">
+      <c r="T30" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - conditioned attic - unvented Residential - mini-split heat pump</v>
       </c>
-      <c r="U30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U30" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="8"/>
         <v>30</v>
@@ -3277,19 +3354,19 @@
       <c r="Q31" s="7">
         <v>2000</v>
       </c>
-      <c r="S31">
+      <c r="S31" s="8">
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="T31" t="str">
+      <c r="T31" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily ambient attic - unvented Residential - ground-to-air heat pump</v>
       </c>
-      <c r="U31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U31" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="8"/>
         <v>31</v>
@@ -3348,19 +3425,22 @@
       <c r="Q32" s="7">
         <v>600</v>
       </c>
-      <c r="S32">
+      <c r="S32" s="8">
         <f t="shared" si="6"/>
         <v>31</v>
       </c>
-      <c r="T32" t="str">
+      <c r="T32" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - vented attic - conditioned Residential - electric resistance and no cooling</v>
       </c>
-      <c r="U32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U32" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="8"/>
         <v>32</v>
@@ -3419,19 +3499,19 @@
       <c r="Q33" s="7">
         <v>800</v>
       </c>
-      <c r="S33">
+      <c r="S33" s="8">
         <f t="shared" si="6"/>
         <v>32</v>
       </c>
-      <c r="T33" t="str">
+      <c r="T33" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - unvented attic - conditioned Residential - electric resistance and central air conditioner</v>
       </c>
-      <c r="U33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U33" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="8"/>
         <v>33</v>
@@ -3490,19 +3570,22 @@
       <c r="Q34" s="7">
         <v>1000</v>
       </c>
-      <c r="S34">
+      <c r="S34" s="8">
         <f t="shared" si="6"/>
         <v>33</v>
       </c>
-      <c r="T34" t="str">
+      <c r="T34" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - unconditioned attic - conditioned Residential - electric resistance and room air conditioner</v>
       </c>
-      <c r="U34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U34" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="8"/>
         <v>34</v>
@@ -3561,19 +3644,19 @@
       <c r="Q35" s="7">
         <v>1500</v>
       </c>
-      <c r="S35">
+      <c r="S35" s="8">
         <f t="shared" si="6"/>
         <v>34</v>
       </c>
-      <c r="T35" t="str">
+      <c r="T35" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - conditioned attic - conditioned Residential - electric resistance and evaporative cooler</v>
       </c>
-      <c r="U35" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U35" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="8"/>
         <v>35</v>
@@ -3632,19 +3715,22 @@
       <c r="Q36" s="7">
         <v>2000</v>
       </c>
-      <c r="S36">
+      <c r="S36" s="8">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
-      <c r="T36" t="str">
+      <c r="T36" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily ambient attic - conditioned Residential - furnace and no cooling</v>
       </c>
-      <c r="U36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U36" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="8"/>
         <v>36</v>
@@ -3703,19 +3789,19 @@
       <c r="Q37" s="7">
         <v>600</v>
       </c>
-      <c r="S37">
+      <c r="S37" s="8">
         <f t="shared" si="6"/>
         <v>36</v>
       </c>
-      <c r="T37" t="str">
+      <c r="T37" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - vented flat roof Residential - furnace and central air conditioner</v>
       </c>
-      <c r="U37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U37" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="8"/>
         <v>37</v>
@@ -3774,19 +3860,22 @@
       <c r="Q38" s="7">
         <v>800</v>
       </c>
-      <c r="S38">
+      <c r="S38" s="8">
         <f t="shared" si="6"/>
         <v>37</v>
       </c>
-      <c r="T38" t="str">
+      <c r="T38" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - unvented flat roof Residential - furnace and room air conditioner</v>
       </c>
-      <c r="U38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U38" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="8"/>
         <v>38</v>
@@ -3845,19 +3934,19 @@
       <c r="Q39" s="7">
         <v>1000</v>
       </c>
-      <c r="S39">
+      <c r="S39" s="8">
         <f t="shared" si="6"/>
         <v>38</v>
       </c>
-      <c r="T39" t="str">
+      <c r="T39" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - unconditioned flat roof Residential - furnace and evaporative cooler</v>
       </c>
-      <c r="U39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U39" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="8"/>
         <v>39</v>
@@ -3916,19 +4005,22 @@
       <c r="Q40" s="7">
         <v>1500</v>
       </c>
-      <c r="S40">
+      <c r="S40" s="8">
         <f t="shared" si="6"/>
         <v>39</v>
       </c>
-      <c r="T40" t="str">
+      <c r="T40" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - conditioned flat roof Residential - boiler and no cooling</v>
       </c>
-      <c r="U40" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U40" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="8"/>
         <v>40</v>
@@ -3987,19 +4079,19 @@
       <c r="Q41" s="7">
         <v>2000</v>
       </c>
-      <c r="S41">
+      <c r="S41" s="8">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="T41" t="str">
+      <c r="T41" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily ambient flat roof Residential - boiler and central air conditioner</v>
       </c>
-      <c r="U41" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U41" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="8"/>
         <v>41</v>
@@ -4058,19 +4150,22 @@
       <c r="Q42" s="7">
         <v>600</v>
       </c>
-      <c r="S42">
+      <c r="S42" s="8">
         <f t="shared" si="6"/>
         <v>41</v>
       </c>
-      <c r="T42" t="str">
+      <c r="T42" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - vented attic - vented Residential - boiler and room air conditioner</v>
       </c>
-      <c r="U42" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U42" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="8"/>
         <v>42</v>
@@ -4129,19 +4224,19 @@
       <c r="Q43" s="7">
         <v>800</v>
       </c>
-      <c r="S43">
+      <c r="S43" s="8">
         <f t="shared" si="6"/>
         <v>42</v>
       </c>
-      <c r="T43" t="str">
+      <c r="T43" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - unvented attic - vented Residential - boiler and evaporative cooler</v>
       </c>
-      <c r="U43" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U43" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="8"/>
         <v>43</v>
@@ -4200,19 +4295,22 @@
       <c r="Q44" s="7">
         <v>1000</v>
       </c>
-      <c r="S44">
+      <c r="S44" s="8">
         <f t="shared" si="6"/>
         <v>43</v>
       </c>
-      <c r="T44" t="str">
+      <c r="T44" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - unconditioned attic - vented Residential - air-to-air heat pump</v>
       </c>
-      <c r="U44" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U44" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="8"/>
         <v>44</v>
@@ -4271,19 +4369,19 @@
       <c r="Q45" s="7">
         <v>1500</v>
       </c>
-      <c r="S45">
+      <c r="S45" s="8">
         <f t="shared" si="6"/>
         <v>44</v>
       </c>
-      <c r="T45" t="str">
+      <c r="T45" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - conditioned attic - vented Residential - mini-split heat pump</v>
       </c>
-      <c r="U45" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U45" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="8"/>
         <v>45</v>
@@ -4342,19 +4440,19 @@
       <c r="Q46" s="7">
         <v>2000</v>
       </c>
-      <c r="S46">
+      <c r="S46" s="8">
         <f t="shared" si="6"/>
         <v>45</v>
       </c>
-      <c r="T46" t="str">
+      <c r="T46" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily ambient attic - vented Residential - ground-to-air heat pump</v>
       </c>
-      <c r="U46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U46" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="8"/>
         <v>46</v>
@@ -4413,19 +4511,19 @@
       <c r="Q47" s="7">
         <v>600</v>
       </c>
-      <c r="S47">
+      <c r="S47" s="8">
         <f t="shared" si="6"/>
         <v>46</v>
       </c>
-      <c r="T47" t="str">
+      <c r="T47" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - vented attic - unvented Residential - electric resistance and no cooling</v>
       </c>
-      <c r="U47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U47" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="8"/>
         <v>47</v>
@@ -4484,19 +4582,22 @@
       <c r="Q48" s="7">
         <v>800</v>
       </c>
-      <c r="S48">
+      <c r="S48" s="8">
         <f t="shared" si="6"/>
         <v>47</v>
       </c>
-      <c r="T48" t="str">
+      <c r="T48" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - unvented attic - unvented Residential - electric resistance and central air conditioner</v>
       </c>
-      <c r="U48" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U48" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="8"/>
         <v>48</v>
@@ -4555,19 +4656,19 @@
       <c r="Q49" s="7">
         <v>1000</v>
       </c>
-      <c r="S49">
+      <c r="S49" s="8">
         <f t="shared" si="6"/>
         <v>48</v>
       </c>
-      <c r="T49" t="str">
+      <c r="T49" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - unconditioned attic - unvented Residential - electric resistance and room air conditioner</v>
       </c>
-      <c r="U49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U49" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="8"/>
         <v>49</v>
@@ -4626,19 +4727,19 @@
       <c r="Q50" s="7">
         <v>1500</v>
       </c>
-      <c r="S50">
+      <c r="S50" s="8">
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="T50" t="str">
+      <c r="T50" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - conditioned attic - unvented Residential - electric resistance and evaporative cooler</v>
       </c>
-      <c r="U50" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U50" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="8"/>
         <v>50</v>
@@ -4697,19 +4798,19 @@
       <c r="Q51" s="7">
         <v>2000</v>
       </c>
-      <c r="S51">
+      <c r="S51" s="8">
         <f t="shared" si="6"/>
         <v>50</v>
       </c>
-      <c r="T51" t="str">
+      <c r="T51" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily ambient attic - unvented Residential - furnace and no cooling</v>
       </c>
-      <c r="U51" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U51" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="8"/>
         <v>51</v>
@@ -4768,19 +4869,22 @@
       <c r="Q52" s="7">
         <v>600</v>
       </c>
-      <c r="S52">
+      <c r="S52" s="8">
         <f t="shared" si="6"/>
         <v>51</v>
       </c>
-      <c r="T52" t="str">
+      <c r="T52" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - vented attic - conditioned Residential - furnace and central air conditioner</v>
       </c>
-      <c r="U52" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U52" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="8"/>
         <v>52</v>
@@ -4839,19 +4943,19 @@
       <c r="Q53" s="7">
         <v>800</v>
       </c>
-      <c r="S53">
+      <c r="S53" s="8">
         <f t="shared" si="6"/>
         <v>52</v>
       </c>
-      <c r="T53" t="str">
+      <c r="T53" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - unvented attic - conditioned Residential - furnace and room air conditioner</v>
       </c>
-      <c r="U53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U53" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="8"/>
         <v>53</v>
@@ -4910,19 +5014,22 @@
       <c r="Q54" s="7">
         <v>1000</v>
       </c>
-      <c r="S54">
+      <c r="S54" s="8">
         <f t="shared" si="6"/>
         <v>53</v>
       </c>
-      <c r="T54" t="str">
+      <c r="T54" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - unconditioned attic - conditioned Residential - furnace and evaporative cooler</v>
       </c>
-      <c r="U54" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U54" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="8"/>
         <v>54</v>
@@ -4981,19 +5088,19 @@
       <c r="Q55" s="7">
         <v>1500</v>
       </c>
-      <c r="S55">
+      <c r="S55" s="8">
         <f t="shared" si="6"/>
         <v>54</v>
       </c>
-      <c r="T55" t="str">
+      <c r="T55" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - conditioned attic - conditioned Residential - boiler and no cooling</v>
       </c>
-      <c r="U55" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U55" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="8"/>
         <v>55</v>
@@ -5052,19 +5159,22 @@
       <c r="Q56" s="7">
         <v>2000</v>
       </c>
-      <c r="S56">
+      <c r="S56" s="8">
         <f t="shared" si="6"/>
         <v>55</v>
       </c>
-      <c r="T56" t="str">
+      <c r="T56" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily ambient attic - conditioned Residential - boiler and central air conditioner</v>
       </c>
-      <c r="U56" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U56" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="8"/>
         <v>56</v>
@@ -5123,19 +5233,19 @@
       <c r="Q57" s="7">
         <v>600</v>
       </c>
-      <c r="S57">
+      <c r="S57" s="8">
         <f t="shared" si="6"/>
         <v>56</v>
       </c>
-      <c r="T57" t="str">
+      <c r="T57" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - vented flat roof Residential - boiler and room air conditioner</v>
       </c>
-      <c r="U57" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U57" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="8"/>
         <v>57</v>
@@ -5194,19 +5304,22 @@
       <c r="Q58" s="7">
         <v>800</v>
       </c>
-      <c r="S58">
+      <c r="S58" s="8">
         <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="T58" t="str">
+      <c r="T58" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - unvented flat roof Residential - boiler and evaporative cooler</v>
       </c>
-      <c r="U58" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U58" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="8"/>
         <v>58</v>
@@ -5265,19 +5378,19 @@
       <c r="Q59" s="7">
         <v>1000</v>
       </c>
-      <c r="S59">
+      <c r="S59" s="8">
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T59" t="str">
+      <c r="T59" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - unconditioned flat roof Residential - air-to-air heat pump</v>
       </c>
-      <c r="U59" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U59" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" si="8"/>
         <v>59</v>
@@ -5336,19 +5449,22 @@
       <c r="Q60" s="7">
         <v>1500</v>
       </c>
-      <c r="S60">
+      <c r="S60" s="8">
         <f t="shared" si="6"/>
         <v>59</v>
       </c>
-      <c r="T60" t="str">
+      <c r="T60" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - conditioned flat roof Residential - mini-split heat pump</v>
       </c>
-      <c r="U60" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U60" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" si="8"/>
         <v>60</v>
@@ -5407,19 +5523,19 @@
       <c r="Q61" s="7">
         <v>2000</v>
       </c>
-      <c r="S61">
+      <c r="S61" s="8">
         <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="T61" t="str">
+      <c r="T61" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily ambient flat roof Residential - ground-to-air heat pump</v>
       </c>
-      <c r="U61" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U61" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" si="8"/>
         <v>61</v>
@@ -5478,19 +5594,22 @@
       <c r="Q62" s="7">
         <v>600</v>
       </c>
-      <c r="S62">
+      <c r="S62" s="8">
         <f t="shared" si="6"/>
         <v>61</v>
       </c>
-      <c r="T62" t="str">
+      <c r="T62" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - vented attic - vented Residential - electric resistance and no cooling</v>
       </c>
-      <c r="U62" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U62" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" si="8"/>
         <v>62</v>
@@ -5549,19 +5668,19 @@
       <c r="Q63" s="7">
         <v>800</v>
       </c>
-      <c r="S63">
+      <c r="S63" s="8">
         <f t="shared" si="6"/>
         <v>62</v>
       </c>
-      <c r="T63" t="str">
+      <c r="T63" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily crawlspace - unvented attic - vented Residential - electric resistance and central air conditioner</v>
       </c>
-      <c r="U63" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U63" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" si="8"/>
         <v>63</v>
@@ -5620,19 +5739,22 @@
       <c r="Q64" s="7">
         <v>1000</v>
       </c>
-      <c r="S64">
+      <c r="S64" s="8">
         <f t="shared" si="6"/>
         <v>63</v>
       </c>
-      <c r="T64" t="str">
+      <c r="T64" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - unconditioned attic - vented Residential - electric resistance and room air conditioner</v>
       </c>
-      <c r="U64" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U64" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W64" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" si="8"/>
         <v>64</v>
@@ -5691,19 +5813,19 @@
       <c r="Q65" s="7">
         <v>1500</v>
       </c>
-      <c r="S65">
+      <c r="S65" s="8">
         <f t="shared" si="6"/>
         <v>64</v>
       </c>
-      <c r="T65" t="str">
+      <c r="T65" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily basement - conditioned attic - vented Residential - electric resistance and evaporative cooler</v>
       </c>
-      <c r="U65" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U65" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" si="8"/>
         <v>65</v>
@@ -5762,19 +5884,19 @@
       <c r="Q66" s="7">
         <v>2000</v>
       </c>
-      <c r="S66">
+      <c r="S66" s="8">
         <f t="shared" si="6"/>
         <v>65</v>
       </c>
-      <c r="T66" t="str">
+      <c r="T66" s="8" t="str">
         <f t="shared" si="7"/>
         <v>Multifamily ambient attic - vented Residential - furnace and no cooling</v>
       </c>
-      <c r="U66" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U66" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A67">
         <f t="shared" si="8"/>
         <v>66</v>
@@ -5833,19 +5955,19 @@
       <c r="Q67" s="7">
         <v>600</v>
       </c>
-      <c r="S67">
+      <c r="S67" s="8">
         <f t="shared" ref="S67:S130" si="15">A67</f>
         <v>66</v>
       </c>
-      <c r="T67" t="str">
+      <c r="T67" s="8" t="str">
         <f t="shared" ref="T67:T130" si="16">B67</f>
         <v>Multifamily crawlspace - vented attic - unvented Residential - furnace and central air conditioner</v>
       </c>
-      <c r="U67" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U67" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A68">
         <f t="shared" ref="A68:A131" si="17">A67+1</f>
         <v>67</v>
@@ -5904,19 +6026,22 @@
       <c r="Q68" s="7">
         <v>800</v>
       </c>
-      <c r="S68">
+      <c r="S68" s="8">
         <f t="shared" si="15"/>
         <v>67</v>
       </c>
-      <c r="T68" t="str">
+      <c r="T68" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - unvented attic - unvented Residential - furnace and room air conditioner</v>
       </c>
-      <c r="U68" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U68" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A69">
         <f t="shared" si="17"/>
         <v>68</v>
@@ -5975,19 +6100,19 @@
       <c r="Q69" s="7">
         <v>1000</v>
       </c>
-      <c r="S69">
+      <c r="S69" s="8">
         <f t="shared" si="15"/>
         <v>68</v>
       </c>
-      <c r="T69" t="str">
+      <c r="T69" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - unconditioned attic - unvented Residential - furnace and evaporative cooler</v>
       </c>
-      <c r="U69" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U69" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A70">
         <f t="shared" si="17"/>
         <v>69</v>
@@ -6046,19 +6171,19 @@
       <c r="Q70" s="7">
         <v>1500</v>
       </c>
-      <c r="S70">
+      <c r="S70" s="8">
         <f t="shared" si="15"/>
         <v>69</v>
       </c>
-      <c r="T70" t="str">
+      <c r="T70" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - conditioned attic - unvented Residential - boiler and no cooling</v>
       </c>
-      <c r="U70" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U70" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A71">
         <f t="shared" si="17"/>
         <v>70</v>
@@ -6117,19 +6242,19 @@
       <c r="Q71" s="7">
         <v>2000</v>
       </c>
-      <c r="S71">
+      <c r="S71" s="8">
         <f t="shared" si="15"/>
         <v>70</v>
       </c>
-      <c r="T71" t="str">
+      <c r="T71" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily ambient attic - unvented Residential - boiler and central air conditioner</v>
       </c>
-      <c r="U71" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U71" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A72">
         <f t="shared" si="17"/>
         <v>71</v>
@@ -6188,19 +6313,22 @@
       <c r="Q72" s="7">
         <v>600</v>
       </c>
-      <c r="S72">
+      <c r="S72" s="8">
         <f t="shared" si="15"/>
         <v>71</v>
       </c>
-      <c r="T72" t="str">
+      <c r="T72" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - vented attic - conditioned Residential - boiler and room air conditioner</v>
       </c>
-      <c r="U72" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U72" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W72" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A73">
         <f t="shared" si="17"/>
         <v>72</v>
@@ -6259,19 +6387,19 @@
       <c r="Q73" s="7">
         <v>800</v>
       </c>
-      <c r="S73">
+      <c r="S73" s="8">
         <f t="shared" si="15"/>
         <v>72</v>
       </c>
-      <c r="T73" t="str">
+      <c r="T73" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - unvented attic - conditioned Residential - boiler and evaporative cooler</v>
       </c>
-      <c r="U73" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U73" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A74">
         <f t="shared" si="17"/>
         <v>73</v>
@@ -6330,19 +6458,22 @@
       <c r="Q74" s="7">
         <v>1000</v>
       </c>
-      <c r="S74">
+      <c r="S74" s="8">
         <f t="shared" si="15"/>
         <v>73</v>
       </c>
-      <c r="T74" t="str">
+      <c r="T74" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - unconditioned attic - conditioned Residential - air-to-air heat pump</v>
       </c>
-      <c r="U74" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U74" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W74" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A75">
         <f t="shared" si="17"/>
         <v>74</v>
@@ -6401,19 +6532,19 @@
       <c r="Q75" s="7">
         <v>1500</v>
       </c>
-      <c r="S75">
+      <c r="S75" s="8">
         <f t="shared" si="15"/>
         <v>74</v>
       </c>
-      <c r="T75" t="str">
+      <c r="T75" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - conditioned attic - conditioned Residential - mini-split heat pump</v>
       </c>
-      <c r="U75" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U75" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A76">
         <f t="shared" si="17"/>
         <v>75</v>
@@ -6472,19 +6603,22 @@
       <c r="Q76" s="7">
         <v>2000</v>
       </c>
-      <c r="S76">
+      <c r="S76" s="8">
         <f t="shared" si="15"/>
         <v>75</v>
       </c>
-      <c r="T76" t="str">
+      <c r="T76" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily ambient attic - conditioned Residential - ground-to-air heat pump</v>
       </c>
-      <c r="U76" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U76" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W76" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A77">
         <f t="shared" si="17"/>
         <v>76</v>
@@ -6543,19 +6677,19 @@
       <c r="Q77" s="7">
         <v>600</v>
       </c>
-      <c r="S77">
+      <c r="S77" s="8">
         <f t="shared" si="15"/>
         <v>76</v>
       </c>
-      <c r="T77" t="str">
+      <c r="T77" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - vented flat roof Residential - electric resistance and no cooling</v>
       </c>
-      <c r="U77" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U77" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A78">
         <f t="shared" si="17"/>
         <v>77</v>
@@ -6614,19 +6748,22 @@
       <c r="Q78" s="7">
         <v>800</v>
       </c>
-      <c r="S78">
+      <c r="S78" s="8">
         <f t="shared" si="15"/>
         <v>77</v>
       </c>
-      <c r="T78" t="str">
+      <c r="T78" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - unvented flat roof Residential - electric resistance and central air conditioner</v>
       </c>
-      <c r="U78" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U78" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W78" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A79">
         <f t="shared" si="17"/>
         <v>78</v>
@@ -6685,19 +6822,19 @@
       <c r="Q79" s="7">
         <v>1000</v>
       </c>
-      <c r="S79">
+      <c r="S79" s="8">
         <f t="shared" si="15"/>
         <v>78</v>
       </c>
-      <c r="T79" t="str">
+      <c r="T79" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - unconditioned flat roof Residential - electric resistance and room air conditioner</v>
       </c>
-      <c r="U79" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U79" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A80">
         <f t="shared" si="17"/>
         <v>79</v>
@@ -6756,19 +6893,22 @@
       <c r="Q80" s="7">
         <v>1500</v>
       </c>
-      <c r="S80">
+      <c r="S80" s="8">
         <f t="shared" si="15"/>
         <v>79</v>
       </c>
-      <c r="T80" t="str">
+      <c r="T80" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - conditioned flat roof Residential - electric resistance and evaporative cooler</v>
       </c>
-      <c r="U80" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U80" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W80" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A81">
         <f t="shared" si="17"/>
         <v>80</v>
@@ -6827,19 +6967,19 @@
       <c r="Q81" s="7">
         <v>2000</v>
       </c>
-      <c r="S81">
+      <c r="S81" s="8">
         <f t="shared" si="15"/>
         <v>80</v>
       </c>
-      <c r="T81" t="str">
+      <c r="T81" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily ambient flat roof Residential - furnace and no cooling</v>
       </c>
-      <c r="U81" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U81" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A82">
         <f t="shared" si="17"/>
         <v>81</v>
@@ -6898,19 +7038,22 @@
       <c r="Q82" s="7">
         <v>600</v>
       </c>
-      <c r="S82">
+      <c r="S82" s="8">
         <f t="shared" si="15"/>
         <v>81</v>
       </c>
-      <c r="T82" t="str">
+      <c r="T82" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - vented attic - vented Residential - furnace and central air conditioner</v>
       </c>
-      <c r="U82" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U82" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W82" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A83">
         <f t="shared" si="17"/>
         <v>82</v>
@@ -6969,19 +7112,19 @@
       <c r="Q83" s="7">
         <v>800</v>
       </c>
-      <c r="S83">
+      <c r="S83" s="8">
         <f t="shared" si="15"/>
         <v>82</v>
       </c>
-      <c r="T83" t="str">
+      <c r="T83" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - unvented attic - vented Residential - furnace and room air conditioner</v>
       </c>
-      <c r="U83" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U83" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A84">
         <f t="shared" si="17"/>
         <v>83</v>
@@ -7040,19 +7183,22 @@
       <c r="Q84" s="7">
         <v>1000</v>
       </c>
-      <c r="S84">
+      <c r="S84" s="8">
         <f t="shared" si="15"/>
         <v>83</v>
       </c>
-      <c r="T84" t="str">
+      <c r="T84" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - unconditioned attic - vented Residential - furnace and evaporative cooler</v>
       </c>
-      <c r="U84" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U84" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W84" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A85">
         <f t="shared" si="17"/>
         <v>84</v>
@@ -7111,19 +7257,19 @@
       <c r="Q85" s="7">
         <v>1500</v>
       </c>
-      <c r="S85">
+      <c r="S85" s="8">
         <f t="shared" si="15"/>
         <v>84</v>
       </c>
-      <c r="T85" t="str">
+      <c r="T85" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - conditioned attic - vented Residential - boiler and no cooling</v>
       </c>
-      <c r="U85" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U85" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A86">
         <f t="shared" si="17"/>
         <v>85</v>
@@ -7182,19 +7328,19 @@
       <c r="Q86" s="7">
         <v>2000</v>
       </c>
-      <c r="S86">
+      <c r="S86" s="8">
         <f t="shared" si="15"/>
         <v>85</v>
       </c>
-      <c r="T86" t="str">
+      <c r="T86" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily ambient attic - vented Residential - boiler and central air conditioner</v>
       </c>
-      <c r="U86" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U86" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A87">
         <f t="shared" si="17"/>
         <v>86</v>
@@ -7253,19 +7399,19 @@
       <c r="Q87" s="7">
         <v>600</v>
       </c>
-      <c r="S87">
+      <c r="S87" s="8">
         <f t="shared" si="15"/>
         <v>86</v>
       </c>
-      <c r="T87" t="str">
+      <c r="T87" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - vented attic - unvented Residential - boiler and room air conditioner</v>
       </c>
-      <c r="U87" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U87" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A88">
         <f t="shared" si="17"/>
         <v>87</v>
@@ -7324,19 +7470,22 @@
       <c r="Q88" s="7">
         <v>800</v>
       </c>
-      <c r="S88">
+      <c r="S88" s="8">
         <f t="shared" si="15"/>
         <v>87</v>
       </c>
-      <c r="T88" t="str">
+      <c r="T88" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - unvented attic - unvented Residential - boiler and evaporative cooler</v>
       </c>
-      <c r="U88" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U88" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W88" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A89">
         <f t="shared" si="17"/>
         <v>88</v>
@@ -7395,19 +7544,19 @@
       <c r="Q89" s="7">
         <v>1000</v>
       </c>
-      <c r="S89">
+      <c r="S89" s="8">
         <f t="shared" si="15"/>
         <v>88</v>
       </c>
-      <c r="T89" t="str">
+      <c r="T89" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - unconditioned attic - unvented Residential - air-to-air heat pump</v>
       </c>
-      <c r="U89" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U89" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A90">
         <f t="shared" si="17"/>
         <v>89</v>
@@ -7466,19 +7615,19 @@
       <c r="Q90" s="7">
         <v>1500</v>
       </c>
-      <c r="S90">
+      <c r="S90" s="8">
         <f t="shared" si="15"/>
         <v>89</v>
       </c>
-      <c r="T90" t="str">
+      <c r="T90" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - conditioned attic - unvented Residential - mini-split heat pump</v>
       </c>
-      <c r="U90" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U90" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A91">
         <f t="shared" si="17"/>
         <v>90</v>
@@ -7537,19 +7686,19 @@
       <c r="Q91" s="7">
         <v>2000</v>
       </c>
-      <c r="S91">
+      <c r="S91" s="8">
         <f t="shared" si="15"/>
         <v>90</v>
       </c>
-      <c r="T91" t="str">
+      <c r="T91" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily ambient attic - unvented Residential - ground-to-air heat pump</v>
       </c>
-      <c r="U91" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U91" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A92">
         <f t="shared" si="17"/>
         <v>91</v>
@@ -7608,19 +7757,22 @@
       <c r="Q92" s="7">
         <v>600</v>
       </c>
-      <c r="S92">
+      <c r="S92" s="8">
         <f t="shared" si="15"/>
         <v>91</v>
       </c>
-      <c r="T92" t="str">
+      <c r="T92" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - vented attic - conditioned Residential - electric resistance and no cooling</v>
       </c>
-      <c r="U92" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U92" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W92" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A93">
         <f t="shared" si="17"/>
         <v>92</v>
@@ -7679,19 +7831,19 @@
       <c r="Q93" s="7">
         <v>800</v>
       </c>
-      <c r="S93">
+      <c r="S93" s="8">
         <f t="shared" si="15"/>
         <v>92</v>
       </c>
-      <c r="T93" t="str">
+      <c r="T93" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - unvented attic - conditioned Residential - electric resistance and central air conditioner</v>
       </c>
-      <c r="U93" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U93" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A94">
         <f t="shared" si="17"/>
         <v>93</v>
@@ -7750,19 +7902,22 @@
       <c r="Q94" s="7">
         <v>1000</v>
       </c>
-      <c r="S94">
+      <c r="S94" s="8">
         <f t="shared" si="15"/>
         <v>93</v>
       </c>
-      <c r="T94" t="str">
+      <c r="T94" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - unconditioned attic - conditioned Residential - electric resistance and room air conditioner</v>
       </c>
-      <c r="U94" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U94" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W94" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" si="17"/>
         <v>94</v>
@@ -7821,19 +7976,19 @@
       <c r="Q95" s="7">
         <v>1500</v>
       </c>
-      <c r="S95">
+      <c r="S95" s="8">
         <f t="shared" si="15"/>
         <v>94</v>
       </c>
-      <c r="T95" t="str">
+      <c r="T95" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - conditioned attic - conditioned Residential - electric resistance and evaporative cooler</v>
       </c>
-      <c r="U95" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U95" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" si="17"/>
         <v>95</v>
@@ -7892,19 +8047,22 @@
       <c r="Q96" s="7">
         <v>2000</v>
       </c>
-      <c r="S96">
+      <c r="S96" s="8">
         <f t="shared" si="15"/>
         <v>95</v>
       </c>
-      <c r="T96" t="str">
+      <c r="T96" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily ambient attic - conditioned Residential - furnace and no cooling</v>
       </c>
-      <c r="U96" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U96" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W96" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" si="17"/>
         <v>96</v>
@@ -7963,19 +8121,19 @@
       <c r="Q97" s="7">
         <v>600</v>
       </c>
-      <c r="S97">
+      <c r="S97" s="8">
         <f t="shared" si="15"/>
         <v>96</v>
       </c>
-      <c r="T97" t="str">
+      <c r="T97" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - vented flat roof Residential - furnace and central air conditioner</v>
       </c>
-      <c r="U97" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U97" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A98">
         <f t="shared" si="17"/>
         <v>97</v>
@@ -8034,19 +8192,22 @@
       <c r="Q98" s="7">
         <v>800</v>
       </c>
-      <c r="S98">
+      <c r="S98" s="8">
         <f t="shared" si="15"/>
         <v>97</v>
       </c>
-      <c r="T98" t="str">
+      <c r="T98" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - unvented flat roof Residential - furnace and room air conditioner</v>
       </c>
-      <c r="U98" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U98" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W98" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A99">
         <f t="shared" si="17"/>
         <v>98</v>
@@ -8105,19 +8266,19 @@
       <c r="Q99" s="7">
         <v>1000</v>
       </c>
-      <c r="S99">
+      <c r="S99" s="8">
         <f t="shared" si="15"/>
         <v>98</v>
       </c>
-      <c r="T99" t="str">
+      <c r="T99" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - unconditioned flat roof Residential - furnace and evaporative cooler</v>
       </c>
-      <c r="U99" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U99" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A100">
         <f t="shared" si="17"/>
         <v>99</v>
@@ -8176,19 +8337,22 @@
       <c r="Q100" s="7">
         <v>1500</v>
       </c>
-      <c r="S100">
+      <c r="S100" s="8">
         <f t="shared" si="15"/>
         <v>99</v>
       </c>
-      <c r="T100" t="str">
+      <c r="T100" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - conditioned flat roof Residential - boiler and no cooling</v>
       </c>
-      <c r="U100" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U100" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W100" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A101">
         <f t="shared" si="17"/>
         <v>100</v>
@@ -8247,19 +8411,19 @@
       <c r="Q101" s="7">
         <v>2000</v>
       </c>
-      <c r="S101">
+      <c r="S101" s="8">
         <f t="shared" si="15"/>
         <v>100</v>
       </c>
-      <c r="T101" t="str">
+      <c r="T101" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily ambient flat roof Residential - boiler and central air conditioner</v>
       </c>
-      <c r="U101" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U101" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A102">
         <f t="shared" si="17"/>
         <v>101</v>
@@ -8318,19 +8482,22 @@
       <c r="Q102" s="7">
         <v>600</v>
       </c>
-      <c r="S102">
+      <c r="S102" s="8">
         <f t="shared" si="15"/>
         <v>101</v>
       </c>
-      <c r="T102" t="str">
+      <c r="T102" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - vented attic - vented Residential - boiler and room air conditioner</v>
       </c>
-      <c r="U102" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U102" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W102" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A103">
         <f t="shared" si="17"/>
         <v>102</v>
@@ -8389,19 +8556,19 @@
       <c r="Q103" s="7">
         <v>800</v>
       </c>
-      <c r="S103">
+      <c r="S103" s="8">
         <f t="shared" si="15"/>
         <v>102</v>
       </c>
-      <c r="T103" t="str">
+      <c r="T103" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - unvented attic - vented Residential - boiler and evaporative cooler</v>
       </c>
-      <c r="U103" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U103" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A104">
         <f t="shared" si="17"/>
         <v>103</v>
@@ -8460,19 +8627,22 @@
       <c r="Q104" s="7">
         <v>1000</v>
       </c>
-      <c r="S104">
+      <c r="S104" s="8">
         <f t="shared" si="15"/>
         <v>103</v>
       </c>
-      <c r="T104" t="str">
+      <c r="T104" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - unconditioned attic - vented Residential - air-to-air heat pump</v>
       </c>
-      <c r="U104" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U104" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W104" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A105">
         <f t="shared" si="17"/>
         <v>104</v>
@@ -8531,19 +8701,19 @@
       <c r="Q105" s="7">
         <v>1500</v>
       </c>
-      <c r="S105">
+      <c r="S105" s="8">
         <f t="shared" si="15"/>
         <v>104</v>
       </c>
-      <c r="T105" t="str">
+      <c r="T105" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - conditioned attic - vented Residential - mini-split heat pump</v>
       </c>
-      <c r="U105" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U105" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A106">
         <f t="shared" si="17"/>
         <v>105</v>
@@ -8602,19 +8772,19 @@
       <c r="Q106" s="7">
         <v>2000</v>
       </c>
-      <c r="S106">
+      <c r="S106" s="8">
         <f t="shared" si="15"/>
         <v>105</v>
       </c>
-      <c r="T106" t="str">
+      <c r="T106" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily ambient attic - vented Residential - ground-to-air heat pump</v>
       </c>
-      <c r="U106" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U106" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A107">
         <f t="shared" si="17"/>
         <v>106</v>
@@ -8673,19 +8843,19 @@
       <c r="Q107" s="7">
         <v>600</v>
       </c>
-      <c r="S107">
+      <c r="S107" s="8">
         <f t="shared" si="15"/>
         <v>106</v>
       </c>
-      <c r="T107" t="str">
+      <c r="T107" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - vented attic - unvented Residential - electric resistance and no cooling</v>
       </c>
-      <c r="U107" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U107" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A108">
         <f t="shared" si="17"/>
         <v>107</v>
@@ -8744,19 +8914,22 @@
       <c r="Q108" s="7">
         <v>800</v>
       </c>
-      <c r="S108">
+      <c r="S108" s="8">
         <f t="shared" si="15"/>
         <v>107</v>
       </c>
-      <c r="T108" t="str">
+      <c r="T108" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - unvented attic - unvented Residential - electric resistance and central air conditioner</v>
       </c>
-      <c r="U108" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U108" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W108" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A109">
         <f t="shared" si="17"/>
         <v>108</v>
@@ -8815,19 +8988,19 @@
       <c r="Q109" s="7">
         <v>1000</v>
       </c>
-      <c r="S109">
+      <c r="S109" s="8">
         <f t="shared" si="15"/>
         <v>108</v>
       </c>
-      <c r="T109" t="str">
+      <c r="T109" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - unconditioned attic - unvented Residential - electric resistance and room air conditioner</v>
       </c>
-      <c r="U109" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U109" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A110">
         <f t="shared" si="17"/>
         <v>109</v>
@@ -8886,19 +9059,19 @@
       <c r="Q110" s="7">
         <v>1500</v>
       </c>
-      <c r="S110">
+      <c r="S110" s="8">
         <f t="shared" si="15"/>
         <v>109</v>
       </c>
-      <c r="T110" t="str">
+      <c r="T110" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - conditioned attic - unvented Residential - electric resistance and evaporative cooler</v>
       </c>
-      <c r="U110" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U110" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="111" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A111">
         <f t="shared" si="17"/>
         <v>110</v>
@@ -8957,19 +9130,19 @@
       <c r="Q111" s="7">
         <v>2000</v>
       </c>
-      <c r="S111">
+      <c r="S111" s="8">
         <f t="shared" si="15"/>
         <v>110</v>
       </c>
-      <c r="T111" t="str">
+      <c r="T111" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily ambient attic - unvented Residential - furnace and no cooling</v>
       </c>
-      <c r="U111" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U111" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="112" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A112">
         <f t="shared" si="17"/>
         <v>111</v>
@@ -9028,19 +9201,22 @@
       <c r="Q112" s="7">
         <v>600</v>
       </c>
-      <c r="S112">
+      <c r="S112" s="8">
         <f t="shared" si="15"/>
         <v>111</v>
       </c>
-      <c r="T112" t="str">
+      <c r="T112" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - vented attic - conditioned Residential - furnace and central air conditioner</v>
       </c>
-      <c r="U112" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U112" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W112" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="113" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A113">
         <f t="shared" si="17"/>
         <v>112</v>
@@ -9099,19 +9275,19 @@
       <c r="Q113" s="7">
         <v>800</v>
       </c>
-      <c r="S113">
+      <c r="S113" s="8">
         <f t="shared" si="15"/>
         <v>112</v>
       </c>
-      <c r="T113" t="str">
+      <c r="T113" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - unvented attic - conditioned Residential - furnace and room air conditioner</v>
       </c>
-      <c r="U113" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U113" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="114" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A114">
         <f t="shared" si="17"/>
         <v>113</v>
@@ -9170,19 +9346,22 @@
       <c r="Q114" s="7">
         <v>1000</v>
       </c>
-      <c r="S114">
+      <c r="S114" s="8">
         <f t="shared" si="15"/>
         <v>113</v>
       </c>
-      <c r="T114" t="str">
+      <c r="T114" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - unconditioned attic - conditioned Residential - furnace and evaporative cooler</v>
       </c>
-      <c r="U114" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U114" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W114" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="115" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A115">
         <f t="shared" si="17"/>
         <v>114</v>
@@ -9241,19 +9420,19 @@
       <c r="Q115" s="7">
         <v>1500</v>
       </c>
-      <c r="S115">
+      <c r="S115" s="8">
         <f t="shared" si="15"/>
         <v>114</v>
       </c>
-      <c r="T115" t="str">
+      <c r="T115" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - conditioned attic - conditioned Residential - boiler and no cooling</v>
       </c>
-      <c r="U115" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U115" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="116" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A116">
         <f t="shared" si="17"/>
         <v>115</v>
@@ -9312,19 +9491,22 @@
       <c r="Q116" s="7">
         <v>2000</v>
       </c>
-      <c r="S116">
+      <c r="S116" s="8">
         <f t="shared" si="15"/>
         <v>115</v>
       </c>
-      <c r="T116" t="str">
+      <c r="T116" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily ambient attic - conditioned Residential - boiler and central air conditioner</v>
       </c>
-      <c r="U116" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U116" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W116" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="117" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A117">
         <f t="shared" si="17"/>
         <v>116</v>
@@ -9383,19 +9565,19 @@
       <c r="Q117" s="7">
         <v>600</v>
       </c>
-      <c r="S117">
+      <c r="S117" s="8">
         <f t="shared" si="15"/>
         <v>116</v>
       </c>
-      <c r="T117" t="str">
+      <c r="T117" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - vented flat roof Residential - boiler and room air conditioner</v>
       </c>
-      <c r="U117" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U117" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="118" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A118">
         <f t="shared" si="17"/>
         <v>117</v>
@@ -9454,19 +9636,22 @@
       <c r="Q118" s="7">
         <v>800</v>
       </c>
-      <c r="S118">
+      <c r="S118" s="8">
         <f t="shared" si="15"/>
         <v>117</v>
       </c>
-      <c r="T118" t="str">
+      <c r="T118" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - unvented flat roof Residential - boiler and evaporative cooler</v>
       </c>
-      <c r="U118" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U118" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W118" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="119" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A119">
         <f t="shared" si="17"/>
         <v>118</v>
@@ -9525,19 +9710,19 @@
       <c r="Q119" s="7">
         <v>1000</v>
       </c>
-      <c r="S119">
+      <c r="S119" s="8">
         <f t="shared" si="15"/>
         <v>118</v>
       </c>
-      <c r="T119" t="str">
+      <c r="T119" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - unconditioned flat roof Residential - air-to-air heat pump</v>
       </c>
-      <c r="U119" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U119" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="120" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A120">
         <f t="shared" si="17"/>
         <v>119</v>
@@ -9596,19 +9781,22 @@
       <c r="Q120" s="7">
         <v>1500</v>
       </c>
-      <c r="S120">
+      <c r="S120" s="8">
         <f t="shared" si="15"/>
         <v>119</v>
       </c>
-      <c r="T120" t="str">
+      <c r="T120" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - conditioned flat roof Residential - mini-split heat pump</v>
       </c>
-      <c r="U120" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U120" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W120" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="121" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A121">
         <f t="shared" si="17"/>
         <v>120</v>
@@ -9667,19 +9855,19 @@
       <c r="Q121" s="7">
         <v>2000</v>
       </c>
-      <c r="S121">
+      <c r="S121" s="8">
         <f t="shared" si="15"/>
         <v>120</v>
       </c>
-      <c r="T121" t="str">
+      <c r="T121" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily ambient flat roof Residential - ground-to-air heat pump</v>
       </c>
-      <c r="U121" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U121" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="122" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A122">
         <f t="shared" si="17"/>
         <v>121</v>
@@ -9738,19 +9926,22 @@
       <c r="Q122" s="7">
         <v>600</v>
       </c>
-      <c r="S122">
+      <c r="S122" s="8">
         <f t="shared" si="15"/>
         <v>121</v>
       </c>
-      <c r="T122" t="str">
+      <c r="T122" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - vented attic - vented Residential - electric resistance and no cooling</v>
       </c>
-      <c r="U122" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U122" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W122" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="123" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A123">
         <f t="shared" si="17"/>
         <v>122</v>
@@ -9809,19 +10000,19 @@
       <c r="Q123" s="7">
         <v>800</v>
       </c>
-      <c r="S123">
+      <c r="S123" s="8">
         <f t="shared" si="15"/>
         <v>122</v>
       </c>
-      <c r="T123" t="str">
+      <c r="T123" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - unvented attic - vented Residential - electric resistance and central air conditioner</v>
       </c>
-      <c r="U123" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U123" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="124" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A124">
         <f t="shared" si="17"/>
         <v>123</v>
@@ -9880,19 +10071,22 @@
       <c r="Q124" s="7">
         <v>1000</v>
       </c>
-      <c r="S124">
+      <c r="S124" s="8">
         <f t="shared" si="15"/>
         <v>123</v>
       </c>
-      <c r="T124" t="str">
+      <c r="T124" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - unconditioned attic - vented Residential - electric resistance and room air conditioner</v>
       </c>
-      <c r="U124" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U124" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W124" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="125" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A125">
         <f t="shared" si="17"/>
         <v>124</v>
@@ -9951,19 +10145,19 @@
       <c r="Q125" s="7">
         <v>1500</v>
       </c>
-      <c r="S125">
+      <c r="S125" s="8">
         <f t="shared" si="15"/>
         <v>124</v>
       </c>
-      <c r="T125" t="str">
+      <c r="T125" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - conditioned attic - vented Residential - electric resistance and evaporative cooler</v>
       </c>
-      <c r="U125" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U125" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="126" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A126">
         <f t="shared" si="17"/>
         <v>125</v>
@@ -10022,19 +10216,19 @@
       <c r="Q126" s="7">
         <v>2000</v>
       </c>
-      <c r="S126">
+      <c r="S126" s="8">
         <f t="shared" si="15"/>
         <v>125</v>
       </c>
-      <c r="T126" t="str">
+      <c r="T126" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily ambient attic - vented Residential - furnace and no cooling</v>
       </c>
-      <c r="U126" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U126" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="127" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A127">
         <f t="shared" si="17"/>
         <v>126</v>
@@ -10093,19 +10287,19 @@
       <c r="Q127" s="7">
         <v>600</v>
       </c>
-      <c r="S127">
+      <c r="S127" s="8">
         <f t="shared" si="15"/>
         <v>126</v>
       </c>
-      <c r="T127" t="str">
+      <c r="T127" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - vented attic - unvented Residential - furnace and central air conditioner</v>
       </c>
-      <c r="U127" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U127" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="128" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A128">
         <f t="shared" si="17"/>
         <v>127</v>
@@ -10164,19 +10358,22 @@
       <c r="Q128" s="7">
         <v>800</v>
       </c>
-      <c r="S128">
+      <c r="S128" s="8">
         <f t="shared" si="15"/>
         <v>127</v>
       </c>
-      <c r="T128" t="str">
+      <c r="T128" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily crawlspace - unvented attic - unvented Residential - furnace and room air conditioner</v>
       </c>
-      <c r="U128" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U128" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W128" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="129" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A129">
         <f t="shared" si="17"/>
         <v>128</v>
@@ -10235,19 +10432,19 @@
       <c r="Q129" s="7">
         <v>1000</v>
       </c>
-      <c r="S129">
+      <c r="S129" s="8">
         <f t="shared" si="15"/>
         <v>128</v>
       </c>
-      <c r="T129" t="str">
+      <c r="T129" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - unconditioned attic - unvented Residential - furnace and evaporative cooler</v>
       </c>
-      <c r="U129" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U129" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="130" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" si="17"/>
         <v>129</v>
@@ -10306,19 +10503,19 @@
       <c r="Q130" s="7">
         <v>1500</v>
       </c>
-      <c r="S130">
+      <c r="S130" s="8">
         <f t="shared" si="15"/>
         <v>129</v>
       </c>
-      <c r="T130" t="str">
+      <c r="T130" s="8" t="str">
         <f t="shared" si="16"/>
         <v>Multifamily basement - conditioned attic - unvented Residential - boiler and no cooling</v>
       </c>
-      <c r="U130" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U130" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="131" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A131">
         <f t="shared" si="17"/>
         <v>130</v>
@@ -10377,19 +10574,19 @@
       <c r="Q131" s="7">
         <v>2000</v>
       </c>
-      <c r="S131">
+      <c r="S131" s="8">
         <f t="shared" ref="S131:S166" si="24">A131</f>
         <v>130</v>
       </c>
-      <c r="T131" t="str">
+      <c r="T131" s="8" t="str">
         <f t="shared" ref="T131:T166" si="25">B131</f>
         <v>Multifamily ambient attic - unvented Residential - boiler and central air conditioner</v>
       </c>
-      <c r="U131" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U131" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="132" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A132">
         <f t="shared" ref="A132:A166" si="26">A131+1</f>
         <v>131</v>
@@ -10448,19 +10645,22 @@
       <c r="Q132" s="7">
         <v>600</v>
       </c>
-      <c r="S132">
+      <c r="S132" s="8">
         <f t="shared" si="24"/>
         <v>131</v>
       </c>
-      <c r="T132" t="str">
+      <c r="T132" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Multifamily crawlspace - vented attic - conditioned Residential - boiler and room air conditioner</v>
       </c>
-      <c r="U132" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U132" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W132" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="133" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A133">
         <f t="shared" si="26"/>
         <v>132</v>
@@ -10519,19 +10719,19 @@
       <c r="Q133" s="7">
         <v>800</v>
       </c>
-      <c r="S133">
+      <c r="S133" s="8">
         <f t="shared" si="24"/>
         <v>132</v>
       </c>
-      <c r="T133" t="str">
+      <c r="T133" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Multifamily crawlspace - unvented attic - conditioned Residential - boiler and evaporative cooler</v>
       </c>
-      <c r="U133" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U133" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="134" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A134">
         <f t="shared" si="26"/>
         <v>133</v>
@@ -10590,19 +10790,22 @@
       <c r="Q134" s="7">
         <v>1000</v>
       </c>
-      <c r="S134">
+      <c r="S134" s="8">
         <f t="shared" si="24"/>
         <v>133</v>
       </c>
-      <c r="T134" t="str">
+      <c r="T134" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Multifamily basement - unconditioned attic - conditioned Residential - air-to-air heat pump</v>
       </c>
-      <c r="U134" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U134" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W134" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="135" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A135">
         <f t="shared" si="26"/>
         <v>134</v>
@@ -10661,19 +10864,19 @@
       <c r="Q135" s="7">
         <v>1500</v>
       </c>
-      <c r="S135">
+      <c r="S135" s="8">
         <f t="shared" si="24"/>
         <v>134</v>
       </c>
-      <c r="T135" t="str">
+      <c r="T135" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Multifamily basement - conditioned attic - conditioned Residential - mini-split heat pump</v>
       </c>
-      <c r="U135" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U135" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="136" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A136">
         <f t="shared" si="26"/>
         <v>135</v>
@@ -10732,19 +10935,22 @@
       <c r="Q136" s="7">
         <v>2000</v>
       </c>
-      <c r="S136">
+      <c r="S136" s="8">
         <f t="shared" si="24"/>
         <v>135</v>
       </c>
-      <c r="T136" t="str">
+      <c r="T136" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Multifamily ambient attic - conditioned Residential - ground-to-air heat pump</v>
       </c>
-      <c r="U136" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U136" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W136" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="137" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A137">
         <f t="shared" si="26"/>
         <v>136</v>
@@ -10803,19 +11009,22 @@
       <c r="Q137" s="7">
         <v>600</v>
       </c>
-      <c r="S137">
+      <c r="S137" s="8">
         <f t="shared" si="24"/>
         <v>136</v>
       </c>
-      <c r="T137" t="str">
+      <c r="T137" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached crawlspace - vented attic - vented Residential - electric resistance and no cooling</v>
       </c>
-      <c r="U137" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U137" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W137" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="138" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A138">
         <f t="shared" si="26"/>
         <v>137</v>
@@ -10874,19 +11083,22 @@
       <c r="Q138" s="7">
         <v>800</v>
       </c>
-      <c r="S138">
+      <c r="S138" s="8">
         <f t="shared" si="24"/>
         <v>137</v>
       </c>
-      <c r="T138" t="str">
+      <c r="T138" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached crawlspace - unvented attic - vented Residential - electric resistance and central air conditioner</v>
       </c>
-      <c r="U138" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U138" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W138" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="139" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A139">
         <f t="shared" si="26"/>
         <v>138</v>
@@ -10945,19 +11157,22 @@
       <c r="Q139" s="7">
         <v>1000</v>
       </c>
-      <c r="S139">
+      <c r="S139" s="8">
         <f t="shared" si="24"/>
         <v>138</v>
       </c>
-      <c r="T139" t="str">
+      <c r="T139" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached basement - unconditioned attic - vented Residential - electric resistance and room air conditioner</v>
       </c>
-      <c r="U139" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U139" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W139" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="140" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A140">
         <f t="shared" si="26"/>
         <v>139</v>
@@ -11016,19 +11231,22 @@
       <c r="Q140" s="7">
         <v>1500</v>
       </c>
-      <c r="S140">
+      <c r="S140" s="8">
         <f t="shared" si="24"/>
         <v>139</v>
       </c>
-      <c r="T140" t="str">
+      <c r="T140" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached basement - conditioned attic - vented Residential - electric resistance and evaporative cooler</v>
       </c>
-      <c r="U140" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U140" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W140" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="141" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A141">
         <f t="shared" si="26"/>
         <v>140</v>
@@ -11087,19 +11305,22 @@
       <c r="Q141" s="7">
         <v>2000</v>
       </c>
-      <c r="S141">
+      <c r="S141" s="8">
         <f t="shared" si="24"/>
         <v>140</v>
       </c>
-      <c r="T141" t="str">
+      <c r="T141" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached ambient attic - vented Residential - furnace and no cooling</v>
       </c>
-      <c r="U141" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U141" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W141" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="142" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A142">
         <f t="shared" si="26"/>
         <v>141</v>
@@ -11158,19 +11379,22 @@
       <c r="Q142" s="7">
         <v>600</v>
       </c>
-      <c r="S142">
+      <c r="S142" s="8">
         <f t="shared" si="24"/>
         <v>141</v>
       </c>
-      <c r="T142" t="str">
+      <c r="T142" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached crawlspace - vented attic - unvented Residential - furnace and central air conditioner</v>
       </c>
-      <c r="U142" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U142" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W142" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="143" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A143">
         <f t="shared" si="26"/>
         <v>142</v>
@@ -11229,19 +11453,22 @@
       <c r="Q143" s="7">
         <v>800</v>
       </c>
-      <c r="S143">
+      <c r="S143" s="8">
         <f t="shared" si="24"/>
         <v>142</v>
       </c>
-      <c r="T143" t="str">
+      <c r="T143" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached crawlspace - unvented attic - unvented Residential - furnace and room air conditioner</v>
       </c>
-      <c r="U143" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U143" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W143" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="144" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A144">
         <f t="shared" si="26"/>
         <v>143</v>
@@ -11300,19 +11527,22 @@
       <c r="Q144" s="7">
         <v>1000</v>
       </c>
-      <c r="S144">
+      <c r="S144" s="8">
         <f t="shared" si="24"/>
         <v>143</v>
       </c>
-      <c r="T144" t="str">
+      <c r="T144" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached basement - unconditioned attic - unvented Residential - furnace and evaporative cooler</v>
       </c>
-      <c r="U144" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="145" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U144" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W144" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="145" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A145">
         <f t="shared" si="26"/>
         <v>144</v>
@@ -11371,19 +11601,22 @@
       <c r="Q145" s="7">
         <v>1500</v>
       </c>
-      <c r="S145">
+      <c r="S145" s="8">
         <f t="shared" si="24"/>
         <v>144</v>
       </c>
-      <c r="T145" t="str">
+      <c r="T145" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached basement - conditioned attic - unvented Residential - boiler and no cooling</v>
       </c>
-      <c r="U145" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="146" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U145" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W145" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="146" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A146">
         <f t="shared" si="26"/>
         <v>145</v>
@@ -11442,19 +11675,22 @@
       <c r="Q146" s="7">
         <v>2000</v>
       </c>
-      <c r="S146">
+      <c r="S146" s="8">
         <f t="shared" si="24"/>
         <v>145</v>
       </c>
-      <c r="T146" t="str">
+      <c r="T146" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached ambient attic - unvented Residential - boiler and central air conditioner</v>
       </c>
-      <c r="U146" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="147" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U146" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W146" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="147" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A147">
         <f t="shared" si="26"/>
         <v>146</v>
@@ -11513,19 +11749,22 @@
       <c r="Q147" s="7">
         <v>600</v>
       </c>
-      <c r="S147">
+      <c r="S147" s="8">
         <f t="shared" si="24"/>
         <v>146</v>
       </c>
-      <c r="T147" t="str">
+      <c r="T147" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached crawlspace - vented attic - conditioned Residential - boiler and room air conditioner</v>
       </c>
-      <c r="U147" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="148" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U147" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W147" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="148" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A148">
         <f t="shared" si="26"/>
         <v>147</v>
@@ -11584,19 +11823,22 @@
       <c r="Q148" s="7">
         <v>800</v>
       </c>
-      <c r="S148">
+      <c r="S148" s="8">
         <f t="shared" si="24"/>
         <v>147</v>
       </c>
-      <c r="T148" t="str">
+      <c r="T148" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached crawlspace - unvented attic - conditioned Residential - boiler and evaporative cooler</v>
       </c>
-      <c r="U148" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="149" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U148" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W148" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="149" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A149">
         <f t="shared" si="26"/>
         <v>148</v>
@@ -11655,19 +11897,22 @@
       <c r="Q149" s="7">
         <v>1000</v>
       </c>
-      <c r="S149">
+      <c r="S149" s="8">
         <f t="shared" si="24"/>
         <v>148</v>
       </c>
-      <c r="T149" t="str">
+      <c r="T149" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached basement - unconditioned attic - conditioned Residential - air-to-air heat pump</v>
       </c>
-      <c r="U149" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="150" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U149" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W149" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="150" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A150">
         <f t="shared" si="26"/>
         <v>149</v>
@@ -11726,19 +11971,22 @@
       <c r="Q150" s="7">
         <v>1500</v>
       </c>
-      <c r="S150">
+      <c r="S150" s="8">
         <f t="shared" si="24"/>
         <v>149</v>
       </c>
-      <c r="T150" t="str">
+      <c r="T150" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached basement - conditioned attic - conditioned Residential - mini-split heat pump</v>
       </c>
-      <c r="U150" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="151" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U150" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W150" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="151" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A151">
         <f t="shared" si="26"/>
         <v>150</v>
@@ -11797,19 +12045,22 @@
       <c r="Q151" s="7">
         <v>2000</v>
       </c>
-      <c r="S151">
+      <c r="S151" s="8">
         <f t="shared" si="24"/>
         <v>150</v>
       </c>
-      <c r="T151" t="str">
+      <c r="T151" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Attached ambient attic - conditioned Residential - ground-to-air heat pump</v>
       </c>
-      <c r="U151" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="152" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U151" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W151" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="152" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A152">
         <f t="shared" si="26"/>
         <v>151</v>
@@ -11867,19 +12118,22 @@
       <c r="Q152" s="7">
         <v>600</v>
       </c>
-      <c r="S152">
+      <c r="S152" s="8">
         <f t="shared" si="24"/>
         <v>151</v>
       </c>
-      <c r="T152" t="str">
+      <c r="T152" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached crawlspace - vented attic - vented Residential - electric resistance and no cooling</v>
       </c>
-      <c r="U152" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="153" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U152" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W152" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="153" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A153">
         <f t="shared" si="26"/>
         <v>152</v>
@@ -11936,19 +12190,22 @@
       <c r="Q153" s="7">
         <v>800</v>
       </c>
-      <c r="S153">
+      <c r="S153" s="8">
         <f t="shared" si="24"/>
         <v>152</v>
       </c>
-      <c r="T153" t="str">
+      <c r="T153" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached crawlspace - unvented attic - vented Residential - electric resistance and central air conditioner</v>
       </c>
-      <c r="U153" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="154" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U153" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W153" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="154" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A154">
         <f t="shared" si="26"/>
         <v>153</v>
@@ -12005,19 +12262,19 @@
       <c r="Q154" s="7">
         <v>1000</v>
       </c>
-      <c r="S154">
+      <c r="S154" s="8">
         <f t="shared" si="24"/>
         <v>153</v>
       </c>
-      <c r="T154" t="str">
+      <c r="T154" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached basement - unconditioned attic - vented Residential - electric resistance and room air conditioner</v>
       </c>
-      <c r="U154" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="155" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U154" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="155" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A155">
         <f t="shared" si="26"/>
         <v>154</v>
@@ -12075,19 +12332,19 @@
       <c r="Q155" s="7">
         <v>1500</v>
       </c>
-      <c r="S155">
+      <c r="S155" s="8">
         <f t="shared" si="24"/>
         <v>154</v>
       </c>
-      <c r="T155" t="str">
+      <c r="T155" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached basement - conditioned attic - vented Residential - electric resistance and evaporative cooler</v>
       </c>
-      <c r="U155" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="156" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U155" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="156" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A156">
         <f t="shared" si="26"/>
         <v>155</v>
@@ -12145,19 +12402,19 @@
       <c r="Q156" s="7">
         <v>2000</v>
       </c>
-      <c r="S156">
+      <c r="S156" s="8">
         <f t="shared" si="24"/>
         <v>155</v>
       </c>
-      <c r="T156" t="str">
+      <c r="T156" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached ambient attic - vented Residential - furnace and no cooling</v>
       </c>
-      <c r="U156" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="157" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U156" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="157" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A157">
         <f t="shared" si="26"/>
         <v>156</v>
@@ -12215,19 +12472,22 @@
       <c r="Q157" s="7">
         <v>600</v>
       </c>
-      <c r="S157">
+      <c r="S157" s="8">
         <f t="shared" si="24"/>
         <v>156</v>
       </c>
-      <c r="T157" t="str">
+      <c r="T157" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached crawlspace - vented attic - unvented Residential - furnace and central air conditioner</v>
       </c>
-      <c r="U157" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="158" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U157" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W157" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="158" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A158">
         <f t="shared" si="26"/>
         <v>157</v>
@@ -12285,19 +12545,19 @@
       <c r="Q158" s="7">
         <v>800</v>
       </c>
-      <c r="S158">
+      <c r="S158" s="8">
         <f t="shared" si="24"/>
         <v>157</v>
       </c>
-      <c r="T158" t="str">
+      <c r="T158" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached crawlspace - unvented attic - unvented Residential - furnace and room air conditioner</v>
       </c>
-      <c r="U158" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="159" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U158" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="159" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A159">
         <f t="shared" si="26"/>
         <v>158</v>
@@ -12355,19 +12615,19 @@
       <c r="Q159" s="7">
         <v>1000</v>
       </c>
-      <c r="S159">
+      <c r="S159" s="8">
         <f t="shared" si="24"/>
         <v>158</v>
       </c>
-      <c r="T159" t="str">
+      <c r="T159" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached basement - unconditioned attic - unvented Residential - furnace and evaporative cooler</v>
       </c>
-      <c r="U159" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="160" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U159" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="160" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A160">
         <f t="shared" si="26"/>
         <v>159</v>
@@ -12425,19 +12685,19 @@
       <c r="Q160" s="7">
         <v>1500</v>
       </c>
-      <c r="S160">
+      <c r="S160" s="8">
         <f t="shared" si="24"/>
         <v>159</v>
       </c>
-      <c r="T160" t="str">
+      <c r="T160" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached basement - conditioned attic - unvented Residential - boiler and no cooling</v>
       </c>
-      <c r="U160" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U160" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="161" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A161">
         <f t="shared" si="26"/>
         <v>160</v>
@@ -12495,19 +12755,19 @@
       <c r="Q161" s="7">
         <v>2000</v>
       </c>
-      <c r="S161">
+      <c r="S161" s="8">
         <f t="shared" si="24"/>
         <v>160</v>
       </c>
-      <c r="T161" t="str">
+      <c r="T161" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached ambient attic - unvented Residential - boiler and central air conditioner</v>
       </c>
-      <c r="U161" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="162" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U161" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="162" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A162">
         <f t="shared" si="26"/>
         <v>161</v>
@@ -12565,19 +12825,22 @@
       <c r="Q162" s="7">
         <v>600</v>
       </c>
-      <c r="S162">
+      <c r="S162" s="8">
         <f t="shared" si="24"/>
         <v>161</v>
       </c>
-      <c r="T162" t="str">
+      <c r="T162" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached crawlspace - vented attic - conditioned Residential - boiler and room air conditioner</v>
       </c>
-      <c r="U162" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="163" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U162" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W162" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="163" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A163">
         <f t="shared" si="26"/>
         <v>162</v>
@@ -12635,19 +12898,19 @@
       <c r="Q163" s="7">
         <v>800</v>
       </c>
-      <c r="S163">
+      <c r="S163" s="8">
         <f t="shared" si="24"/>
         <v>162</v>
       </c>
-      <c r="T163" t="str">
+      <c r="T163" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached crawlspace - unvented attic - conditioned Residential - boiler and evaporative cooler</v>
       </c>
-      <c r="U163" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="164" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U163" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="164" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A164">
         <f t="shared" si="26"/>
         <v>163</v>
@@ -12705,19 +12968,22 @@
       <c r="Q164" s="7">
         <v>1000</v>
       </c>
-      <c r="S164">
+      <c r="S164" s="8">
         <f t="shared" si="24"/>
         <v>163</v>
       </c>
-      <c r="T164" t="str">
+      <c r="T164" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached basement - unconditioned attic - conditioned Residential - air-to-air heat pump</v>
       </c>
-      <c r="U164" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="165" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U164" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="W164" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="165" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A165">
         <f t="shared" si="26"/>
         <v>164</v>
@@ -12775,19 +13041,19 @@
       <c r="Q165" s="7">
         <v>1500</v>
       </c>
-      <c r="S165">
+      <c r="S165" s="8">
         <f t="shared" si="24"/>
         <v>164</v>
       </c>
-      <c r="T165" t="str">
+      <c r="T165" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached basement - conditioned attic - conditioned Residential - mini-split heat pump</v>
       </c>
-      <c r="U165" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="166" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U165" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="166" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A166">
         <f t="shared" si="26"/>
         <v>165</v>
@@ -12845,19 +13111,29 @@
       <c r="Q166" s="7">
         <v>2000</v>
       </c>
-      <c r="S166">
+      <c r="S166" s="8">
         <f t="shared" si="24"/>
         <v>165</v>
       </c>
-      <c r="T166" t="str">
+      <c r="T166" s="8" t="str">
         <f t="shared" si="25"/>
         <v>Single-Family Detached ambient attic - conditioned Residential - ground-to-air heat pump</v>
       </c>
-      <c r="U166" t="s">
-        <v>57</v>
+      <c r="U166" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="169" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W169">
+        <f>SUBTOTAL(3,W2:W166)</f>
+        <v>74</v>
+      </c>
+      <c r="X169" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:W166" xr:uid="{21B1780A-226A-2041-992F-87E8C445BCFC}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
missing a lot more fields
should all be there now
</commit_message>
<xml_diff>
--- a/example_project/res_testing_inputs.xlsx
+++ b/example_project/res_testing_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgoldwas/Documents/GitHub/URBANopt/urbanopt-example-geojson-project/example_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298273D9-E8C7-F647-A89E-2984CA3D93B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D85F0C3-0F14-8B4C-8AC9-CA884DF87B1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1102,10 +1102,10 @@
   <dimension ref="A1:X169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B123" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C137" sqref="C137"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
saving about error log for half of test run
Other half will finish tonight and I'll update this. Will probably re-run tomorrow.
</commit_message>
<xml_diff>
--- a/example_project/res_testing_inputs.xlsx
+++ b/example_project/res_testing_inputs.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgoldwas/Documents/GitHub/URBANopt/urbanopt-example-geojson-project/example_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D85F0C3-0F14-8B4C-8AC9-CA884DF87B1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C5223D-6EFF-BE4F-9153-093ABFCA77BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="res_testing_inputs" sheetId="1" r:id="rId1"/>
     <sheet name="Inputs Options" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">res_testing_inputs!$A$1:$W$166</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">res_testing_inputs!$A$1:$X$166</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="72">
   <si>
     <t>id</t>
   </si>
@@ -223,10 +223,34 @@
     <t>Number of errors out of 165 simulations</t>
   </si>
   <si>
-    <t>Expected NumberofBedrooms to be less than or equal to (ConditionedFloorArea-120)/70 [context: /HPXML/Building/BuildingDetails/BuildingSummary/BuildingConstruction]</t>
+    <t>TypeError: no implicit conversion from nil to integer (BuildResidentialHPXML/resources/schedules.rb:1078:in )</t>
   </si>
   <si>
-    <t>["The number of units (8) must be divisible by the number of floors (3).", "Unsuccessful creation of HPXML file."]</t>
+    <t>geometry_unit_type=apartment unit and geometry_foundation_type=ConditionedBasement</t>
+  </si>
+  <si>
+    <t>geometry_unit_type=apartment unit and geometry_foundation_type=Ambient</t>
+  </si>
+  <si>
+    <t>TypeError: false can't be coerced into Float (BuildResidentialHPXML/measure.rb:3783)</t>
+  </si>
+  <si>
+    <t>The number of units (64) must be divisible by the number of floors (3)</t>
+  </si>
+  <si>
+    <t>Could not find argument 'heat_pump_heating_efficiency_type=HSPF'</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>geometry_num_floors_above_grade=1 and geometry_attic_type=ConditionedAttic</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Somehow worked with number_of_residential_units which drives other columns empty</t>
   </si>
 </sst>
 </file>
@@ -369,7 +393,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -573,6 +597,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -734,7 +764,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -744,6 +774,7 @@
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1099,13 +1130,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X169"/>
+  <dimension ref="A1:Y169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="W79" sqref="W79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1128,9 +1159,10 @@
     <col min="21" max="21" width="36.1640625" style="8" customWidth="1"/>
     <col min="23" max="23" width="15.6640625" customWidth="1"/>
     <col min="24" max="24" width="86.1640625" customWidth="1"/>
+    <col min="25" max="25" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1197,8 +1229,11 @@
       <c r="X1" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y1" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1270,11 +1305,11 @@
       <c r="W2" t="s">
         <v>59</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1345,7 +1380,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A67" si="8">A3+1</f>
         <v>3</v>
@@ -1415,14 +1450,8 @@
       <c r="U4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W4" t="s">
-        <v>59</v>
-      </c>
-      <c r="X4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="8"/>
         <v>4</v>
@@ -1492,8 +1521,14 @@
       <c r="U5" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W5" t="s">
+        <v>59</v>
+      </c>
+      <c r="X5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="8"/>
         <v>5</v>
@@ -1563,8 +1598,14 @@
       <c r="U6" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W6" t="s">
+        <v>59</v>
+      </c>
+      <c r="X6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="8"/>
         <v>6</v>
@@ -1635,7 +1676,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="8"/>
         <v>7</v>
@@ -1705,11 +1746,8 @@
       <c r="U8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="8"/>
         <v>8</v>
@@ -1780,7 +1818,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="8"/>
         <v>9</v>
@@ -1850,8 +1888,14 @@
       <c r="U10" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W10" t="s">
+        <v>59</v>
+      </c>
+      <c r="X10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="8"/>
         <v>10</v>
@@ -1921,8 +1965,14 @@
       <c r="U11" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W11" t="s">
+        <v>59</v>
+      </c>
+      <c r="X11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="8"/>
         <v>11</v>
@@ -1995,8 +2045,11 @@
       <c r="W12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X12" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="8"/>
         <v>12</v>
@@ -2066,8 +2119,14 @@
       <c r="U13" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W13" t="s">
+        <v>59</v>
+      </c>
+      <c r="X13" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="8"/>
         <v>13</v>
@@ -2140,8 +2199,11 @@
       <c r="W14" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X14" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="8"/>
         <v>14</v>
@@ -2211,8 +2273,14 @@
       <c r="U15" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W15" t="s">
+        <v>59</v>
+      </c>
+      <c r="X15" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="8"/>
         <v>15</v>
@@ -2285,8 +2353,11 @@
       <c r="W16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="8"/>
         <v>16</v>
@@ -2298,13 +2369,13 @@
       <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="3" t="e">
         <f t="shared" si="1"/>
-        <v>115200</v>
-      </c>
-      <c r="E17" s="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E17" s="3" t="e">
         <f t="shared" si="2"/>
-        <v>28800</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F17">
         <v>4</v>
@@ -2313,9 +2384,9 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="3" t="e">
         <f t="shared" si="4"/>
-        <v>192</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I17" t="s">
         <v>41</v>
@@ -2329,9 +2400,8 @@
       <c r="L17" t="s">
         <v>33</v>
       </c>
-      <c r="M17" s="3">
-        <f t="shared" si="5"/>
-        <v>64</v>
+      <c r="M17" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="N17" t="s">
         <v>38</v>
@@ -2356,8 +2426,11 @@
       <c r="U17" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Y17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="8"/>
         <v>17</v>
@@ -2430,8 +2503,11 @@
       <c r="W18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X18" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -2502,7 +2578,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -2575,8 +2651,11 @@
       <c r="W20" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -2646,8 +2725,14 @@
       <c r="U21" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W21" t="s">
+        <v>59</v>
+      </c>
+      <c r="X21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -2720,8 +2805,11 @@
       <c r="W22" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X22" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -2792,7 +2880,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -2862,11 +2950,8 @@
       <c r="U24" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -2936,8 +3021,14 @@
       <c r="U25" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W25" t="s">
+        <v>59</v>
+      </c>
+      <c r="X25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="8"/>
         <v>25</v>
@@ -3007,8 +3098,14 @@
       <c r="U26" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W26" t="s">
+        <v>59</v>
+      </c>
+      <c r="X26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="8"/>
         <v>26</v>
@@ -3079,7 +3176,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="8"/>
         <v>27</v>
@@ -3149,11 +3246,8 @@
       <c r="U28" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="8"/>
         <v>28</v>
@@ -3223,8 +3317,14 @@
       <c r="U29" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W29" t="s">
+        <v>59</v>
+      </c>
+      <c r="X29" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="8"/>
         <v>29</v>
@@ -3294,8 +3394,14 @@
       <c r="U30" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W30" t="s">
+        <v>59</v>
+      </c>
+      <c r="X30" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="8"/>
         <v>30</v>
@@ -3365,8 +3471,14 @@
       <c r="U31" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W31" t="s">
+        <v>59</v>
+      </c>
+      <c r="X31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="8"/>
         <v>31</v>
@@ -3439,8 +3551,11 @@
       <c r="W32" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X32" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="8"/>
         <v>32</v>
@@ -3510,8 +3625,14 @@
       <c r="U33" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W33" t="s">
+        <v>59</v>
+      </c>
+      <c r="X33" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="8"/>
         <v>33</v>
@@ -3584,8 +3705,11 @@
       <c r="W34" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="8"/>
         <v>34</v>
@@ -3655,8 +3779,14 @@
       <c r="U35" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W35" t="s">
+        <v>59</v>
+      </c>
+      <c r="X35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="8"/>
         <v>35</v>
@@ -3729,8 +3859,11 @@
       <c r="W36" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="8"/>
         <v>36</v>
@@ -3801,7 +3934,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="8"/>
         <v>37</v>
@@ -3874,8 +4007,11 @@
       <c r="W38" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X38" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="8"/>
         <v>38</v>
@@ -3946,7 +4082,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="8"/>
         <v>39</v>
@@ -4019,8 +4155,11 @@
       <c r="W40" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="8"/>
         <v>40</v>
@@ -4090,8 +4229,14 @@
       <c r="U41" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W41" t="s">
+        <v>59</v>
+      </c>
+      <c r="X41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="8"/>
         <v>41</v>
@@ -4164,8 +4309,11 @@
       <c r="W42" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X42" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="8"/>
         <v>42</v>
@@ -4236,7 +4384,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="8"/>
         <v>43</v>
@@ -4309,8 +4457,11 @@
       <c r="W44" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X44" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="8"/>
         <v>44</v>
@@ -4380,8 +4531,14 @@
       <c r="U45" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W45" t="s">
+        <v>59</v>
+      </c>
+      <c r="X45" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="8"/>
         <v>45</v>
@@ -4451,8 +4608,14 @@
       <c r="U46" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W46" t="s">
+        <v>59</v>
+      </c>
+      <c r="X46" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="8"/>
         <v>46</v>
@@ -4523,7 +4686,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="8"/>
         <v>47</v>
@@ -4593,11 +4756,8 @@
       <c r="U48" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W48" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="8"/>
         <v>48</v>
@@ -4668,7 +4828,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="8"/>
         <v>49</v>
@@ -4738,8 +4898,14 @@
       <c r="U50" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W50" t="s">
+        <v>59</v>
+      </c>
+      <c r="X50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="8"/>
         <v>50</v>
@@ -4809,8 +4975,14 @@
       <c r="U51" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W51" t="s">
+        <v>59</v>
+      </c>
+      <c r="X51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="8"/>
         <v>51</v>
@@ -4883,8 +5055,11 @@
       <c r="W52" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X52" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="8"/>
         <v>52</v>
@@ -4954,8 +5129,14 @@
       <c r="U53" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W53" t="s">
+        <v>59</v>
+      </c>
+      <c r="X53" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="8"/>
         <v>53</v>
@@ -5028,8 +5209,11 @@
       <c r="W54" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="8"/>
         <v>54</v>
@@ -5099,8 +5283,14 @@
       <c r="U55" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W55" t="s">
+        <v>59</v>
+      </c>
+      <c r="X55" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="8"/>
         <v>55</v>
@@ -5173,8 +5363,11 @@
       <c r="W56" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X56" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="8"/>
         <v>56</v>
@@ -5245,7 +5438,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="8"/>
         <v>57</v>
@@ -5318,8 +5511,11 @@
       <c r="W58" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X58" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="8"/>
         <v>58</v>
@@ -5389,8 +5585,14 @@
       <c r="U59" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W59" t="s">
+        <v>59</v>
+      </c>
+      <c r="X59" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" si="8"/>
         <v>59</v>
@@ -5463,8 +5665,11 @@
       <c r="W60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X60" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" si="8"/>
         <v>60</v>
@@ -5534,8 +5739,14 @@
       <c r="U61" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W61" t="s">
+        <v>59</v>
+      </c>
+      <c r="X61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" si="8"/>
         <v>61</v>
@@ -5608,8 +5819,11 @@
       <c r="W62" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X62" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" si="8"/>
         <v>62</v>
@@ -5680,7 +5894,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" si="8"/>
         <v>63</v>
@@ -5750,11 +5964,8 @@
       <c r="U64" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W64" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" si="8"/>
         <v>64</v>
@@ -5824,8 +6035,14 @@
       <c r="U65" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W65" t="s">
+        <v>59</v>
+      </c>
+      <c r="X65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" si="8"/>
         <v>65</v>
@@ -5895,8 +6112,14 @@
       <c r="U66" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W66" t="s">
+        <v>59</v>
+      </c>
+      <c r="X66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A67">
         <f t="shared" si="8"/>
         <v>66</v>
@@ -5967,7 +6190,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A68">
         <f t="shared" ref="A68:A131" si="17">A67+1</f>
         <v>67</v>
@@ -6037,11 +6260,8 @@
       <c r="U68" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W68" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A69">
         <f t="shared" si="17"/>
         <v>68</v>
@@ -6112,7 +6332,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A70">
         <f t="shared" si="17"/>
         <v>69</v>
@@ -6182,8 +6402,14 @@
       <c r="U70" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W70" t="s">
+        <v>59</v>
+      </c>
+      <c r="X70" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A71">
         <f t="shared" si="17"/>
         <v>70</v>
@@ -6253,8 +6479,14 @@
       <c r="U71" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W71" t="s">
+        <v>59</v>
+      </c>
+      <c r="X71" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A72">
         <f t="shared" si="17"/>
         <v>71</v>
@@ -6327,8 +6559,11 @@
       <c r="W72" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X72" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A73">
         <f t="shared" si="17"/>
         <v>72</v>
@@ -6398,8 +6633,14 @@
       <c r="U73" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W73" t="s">
+        <v>59</v>
+      </c>
+      <c r="X73" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A74">
         <f t="shared" si="17"/>
         <v>73</v>
@@ -6472,8 +6713,11 @@
       <c r="W74" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X74" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A75">
         <f t="shared" si="17"/>
         <v>74</v>
@@ -6543,8 +6787,14 @@
       <c r="U75" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W75" t="s">
+        <v>59</v>
+      </c>
+      <c r="X75" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A76">
         <f t="shared" si="17"/>
         <v>75</v>
@@ -6617,8 +6867,11 @@
       <c r="W76" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X76" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A77">
         <f t="shared" si="17"/>
         <v>76</v>
@@ -6688,8 +6941,9 @@
       <c r="U77" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X77" s="4"/>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A78">
         <f t="shared" si="17"/>
         <v>77</v>
@@ -6759,11 +7013,8 @@
       <c r="U78" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W78" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79">
         <f t="shared" si="17"/>
         <v>78</v>
@@ -6834,7 +7085,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A80">
         <f t="shared" si="17"/>
         <v>79</v>
@@ -6904,11 +7155,8 @@
       <c r="U80" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W80" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A81">
         <f t="shared" si="17"/>
         <v>80</v>
@@ -6979,7 +7227,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A82">
         <f t="shared" si="17"/>
         <v>81</v>
@@ -7049,11 +7297,8 @@
       <c r="U82" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W82" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A83">
         <f t="shared" si="17"/>
         <v>82</v>
@@ -7124,7 +7369,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A84">
         <f t="shared" si="17"/>
         <v>83</v>
@@ -7194,11 +7439,8 @@
       <c r="U84" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W84" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A85">
         <f t="shared" si="17"/>
         <v>84</v>
@@ -7269,7 +7511,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A86">
         <f t="shared" si="17"/>
         <v>85</v>
@@ -7340,7 +7582,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A87">
         <f t="shared" si="17"/>
         <v>86</v>
@@ -7411,7 +7653,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A88">
         <f t="shared" si="17"/>
         <v>87</v>
@@ -7481,11 +7723,8 @@
       <c r="U88" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W88" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A89">
         <f t="shared" si="17"/>
         <v>88</v>
@@ -7556,7 +7795,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A90">
         <f t="shared" si="17"/>
         <v>89</v>
@@ -7627,7 +7866,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A91">
         <f t="shared" si="17"/>
         <v>90</v>
@@ -7698,7 +7937,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A92">
         <f t="shared" si="17"/>
         <v>91</v>
@@ -7768,11 +8007,8 @@
       <c r="U92" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W92" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A93">
         <f t="shared" si="17"/>
         <v>92</v>
@@ -7843,7 +8079,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A94">
         <f t="shared" si="17"/>
         <v>93</v>
@@ -7913,11 +8149,8 @@
       <c r="U94" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W94" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" si="17"/>
         <v>94</v>
@@ -7988,7 +8221,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" si="17"/>
         <v>95</v>
@@ -8058,11 +8291,8 @@
       <c r="U96" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W96" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" si="17"/>
         <v>96</v>
@@ -8133,7 +8363,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A98">
         <f t="shared" si="17"/>
         <v>97</v>
@@ -8203,11 +8433,8 @@
       <c r="U98" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W98" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A99">
         <f t="shared" si="17"/>
         <v>98</v>
@@ -8278,7 +8505,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A100">
         <f t="shared" si="17"/>
         <v>99</v>
@@ -8348,11 +8575,8 @@
       <c r="U100" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W100" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A101">
         <f t="shared" si="17"/>
         <v>100</v>
@@ -8423,7 +8647,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A102">
         <f t="shared" si="17"/>
         <v>101</v>
@@ -8493,11 +8717,8 @@
       <c r="U102" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W102" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A103">
         <f t="shared" si="17"/>
         <v>102</v>
@@ -8568,7 +8789,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A104">
         <f t="shared" si="17"/>
         <v>103</v>
@@ -8638,11 +8859,8 @@
       <c r="U104" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W104" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A105">
         <f t="shared" si="17"/>
         <v>104</v>
@@ -8713,7 +8931,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A106">
         <f t="shared" si="17"/>
         <v>105</v>
@@ -8784,7 +9002,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A107">
         <f t="shared" si="17"/>
         <v>106</v>
@@ -8855,7 +9073,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A108">
         <f t="shared" si="17"/>
         <v>107</v>
@@ -8925,11 +9143,8 @@
       <c r="U108" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W108" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A109">
         <f t="shared" si="17"/>
         <v>108</v>
@@ -9000,7 +9215,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A110">
         <f t="shared" si="17"/>
         <v>109</v>
@@ -9071,7 +9286,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A111">
         <f t="shared" si="17"/>
         <v>110</v>
@@ -9142,7 +9357,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A112">
         <f t="shared" si="17"/>
         <v>111</v>
@@ -9212,11 +9427,8 @@
       <c r="U112" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W112" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A113">
         <f t="shared" si="17"/>
         <v>112</v>
@@ -9287,7 +9499,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A114">
         <f t="shared" si="17"/>
         <v>113</v>
@@ -9357,11 +9569,8 @@
       <c r="U114" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W114" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A115">
         <f t="shared" si="17"/>
         <v>114</v>
@@ -9432,7 +9641,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A116">
         <f t="shared" si="17"/>
         <v>115</v>
@@ -9502,11 +9711,8 @@
       <c r="U116" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W116" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A117">
         <f t="shared" si="17"/>
         <v>116</v>
@@ -9577,7 +9783,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A118">
         <f t="shared" si="17"/>
         <v>117</v>
@@ -9647,11 +9853,8 @@
       <c r="U118" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W118" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A119">
         <f t="shared" si="17"/>
         <v>118</v>
@@ -9722,7 +9925,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A120">
         <f t="shared" si="17"/>
         <v>119</v>
@@ -9792,11 +9995,8 @@
       <c r="U120" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W120" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A121">
         <f t="shared" si="17"/>
         <v>120</v>
@@ -9867,7 +10067,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A122">
         <f t="shared" si="17"/>
         <v>121</v>
@@ -9937,11 +10137,8 @@
       <c r="U122" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W122" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A123">
         <f t="shared" si="17"/>
         <v>122</v>
@@ -10012,7 +10209,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A124">
         <f t="shared" si="17"/>
         <v>123</v>
@@ -10082,11 +10279,8 @@
       <c r="U124" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W124" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A125">
         <f t="shared" si="17"/>
         <v>124</v>
@@ -10157,7 +10351,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A126">
         <f t="shared" si="17"/>
         <v>125</v>
@@ -10228,7 +10422,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A127">
         <f t="shared" si="17"/>
         <v>126</v>
@@ -10299,7 +10493,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A128">
         <f t="shared" si="17"/>
         <v>127</v>
@@ -10369,11 +10563,8 @@
       <c r="U128" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W128" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A129">
         <f t="shared" si="17"/>
         <v>128</v>
@@ -10444,7 +10635,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" si="17"/>
         <v>129</v>
@@ -10515,7 +10706,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A131">
         <f t="shared" si="17"/>
         <v>130</v>
@@ -10586,7 +10777,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A132">
         <f t="shared" ref="A132:A166" si="26">A131+1</f>
         <v>131</v>
@@ -10656,11 +10847,8 @@
       <c r="U132" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W132" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="133" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A133">
         <f t="shared" si="26"/>
         <v>132</v>
@@ -10731,7 +10919,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A134">
         <f t="shared" si="26"/>
         <v>133</v>
@@ -10801,11 +10989,8 @@
       <c r="U134" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W134" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="135" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A135">
         <f t="shared" si="26"/>
         <v>134</v>
@@ -10876,7 +11061,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A136">
         <f t="shared" si="26"/>
         <v>135</v>
@@ -10946,11 +11131,8 @@
       <c r="U136" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W136" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A137">
         <f t="shared" si="26"/>
         <v>136</v>
@@ -11020,11 +11202,8 @@
       <c r="U137" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W137" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="138" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A138">
         <f t="shared" si="26"/>
         <v>137</v>
@@ -11094,11 +11273,8 @@
       <c r="U138" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W138" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="139" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A139">
         <f t="shared" si="26"/>
         <v>138</v>
@@ -11168,11 +11344,8 @@
       <c r="U139" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W139" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="140" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A140">
         <f t="shared" si="26"/>
         <v>139</v>
@@ -11242,11 +11415,8 @@
       <c r="U140" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W140" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="141" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A141">
         <f t="shared" si="26"/>
         <v>140</v>
@@ -11316,11 +11486,8 @@
       <c r="U141" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W141" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="142" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A142">
         <f t="shared" si="26"/>
         <v>141</v>
@@ -11390,11 +11557,8 @@
       <c r="U142" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W142" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="143" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A143">
         <f t="shared" si="26"/>
         <v>142</v>
@@ -11464,11 +11628,8 @@
       <c r="U143" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W143" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="144" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A144">
         <f t="shared" si="26"/>
         <v>143</v>
@@ -11538,11 +11699,8 @@
       <c r="U144" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W144" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="145" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A145">
         <f t="shared" si="26"/>
         <v>144</v>
@@ -11612,11 +11770,8 @@
       <c r="U145" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W145" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="146" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A146">
         <f t="shared" si="26"/>
         <v>145</v>
@@ -11686,11 +11841,8 @@
       <c r="U146" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W146" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="147" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A147">
         <f t="shared" si="26"/>
         <v>146</v>
@@ -11760,11 +11912,8 @@
       <c r="U147" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W147" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A148">
         <f t="shared" si="26"/>
         <v>147</v>
@@ -11834,11 +11983,8 @@
       <c r="U148" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W148" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="149" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A149">
         <f t="shared" si="26"/>
         <v>148</v>
@@ -11908,11 +12054,8 @@
       <c r="U149" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W149" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="150" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A150">
         <f t="shared" si="26"/>
         <v>149</v>
@@ -11982,11 +12125,8 @@
       <c r="U150" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W150" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="151" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A151">
         <f t="shared" si="26"/>
         <v>150</v>
@@ -12056,11 +12196,8 @@
       <c r="U151" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W151" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="152" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A152">
         <f t="shared" si="26"/>
         <v>151</v>
@@ -12129,11 +12266,8 @@
       <c r="U152" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W152" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="153" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A153">
         <f t="shared" si="26"/>
         <v>152</v>
@@ -12201,11 +12335,8 @@
       <c r="U153" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W153" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="154" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A154">
         <f t="shared" si="26"/>
         <v>153</v>
@@ -12274,7 +12405,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A155">
         <f t="shared" si="26"/>
         <v>154</v>
@@ -12344,7 +12475,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A156">
         <f t="shared" si="26"/>
         <v>155</v>
@@ -12414,7 +12545,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A157">
         <f t="shared" si="26"/>
         <v>156</v>
@@ -12483,11 +12614,8 @@
       <c r="U157" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W157" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="158" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A158">
         <f t="shared" si="26"/>
         <v>157</v>
@@ -12557,7 +12685,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A159">
         <f t="shared" si="26"/>
         <v>158</v>
@@ -12627,7 +12755,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A160">
         <f t="shared" si="26"/>
         <v>159</v>
@@ -12836,9 +12964,6 @@
       <c r="U162" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W162" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="163" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A163">
@@ -12979,9 +13104,6 @@
       <c r="U164" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W164" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="165" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A165">
@@ -13126,14 +13248,14 @@
     <row r="169" spans="1:24" x14ac:dyDescent="0.2">
       <c r="W169">
         <f>SUBTOTAL(3,W2:W166)</f>
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="X169" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W166" xr:uid="{21B1780A-226A-2041-992F-87E8C445BCFC}"/>
+  <autoFilter ref="A1:X166" xr:uid="{457AABF6-AAD8-B145-8504-C6C2D8C240CB}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updating run logs in Excel file
few new error types listed including severe errors in E+
</commit_message>
<xml_diff>
--- a/example_project/res_testing_inputs.xlsx
+++ b/example_project/res_testing_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgoldwas/Documents/GitHub/URBANopt/urbanopt-example-geojson-project/example_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C5223D-6EFF-BE4F-9153-093ABFCA77BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AF5F65-9EC3-654A-9978-71AA43784CBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="res_testing_inputs" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="76">
   <si>
     <t>id</t>
   </si>
@@ -252,6 +252,18 @@
   <si>
     <t>Somehow worked with number_of_residential_units which drives other columns empty</t>
   </si>
+  <si>
+    <t>** Severe  ** Problem found in EMS EnergyPlus Runtime Language</t>
+  </si>
+  <si>
+    <t>I need to check closer for other errors like this that I may have missed skimming through results</t>
+  </si>
+  <si>
+    <t>** Severe  ** Plant temperatures are getting far too hot, check controls and relative loads and capacities</t>
+  </si>
+  <si>
+    <t>Expected 1 element(s) for xpath: AnnualCoolingEfficiency[Units="EER" ](HeatPumpType="ground-to-air)</t>
+  </si>
 </sst>
 </file>
 
@@ -393,7 +405,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -603,6 +615,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -764,7 +782,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -775,6 +793,7 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1133,15 +1152,15 @@
   <dimension ref="A1:Y169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W79" sqref="W79"/>
+      <selection pane="bottomRight" activeCell="W4" sqref="W4:X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="48.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="5" width="19" style="3" customWidth="1"/>
@@ -1154,7 +1173,7 @@
     <col min="14" max="14" width="50.33203125" customWidth="1"/>
     <col min="15" max="15" width="31.33203125" style="7" customWidth="1"/>
     <col min="16" max="16" width="21.33203125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="35.83203125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="21.83203125" style="7" customWidth="1"/>
     <col min="19" max="20" width="10.83203125" style="8"/>
     <col min="21" max="21" width="36.1640625" style="8" customWidth="1"/>
     <col min="23" max="23" width="15.6640625" customWidth="1"/>
@@ -1450,6 +1469,12 @@
       <c r="U4" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W4" t="s">
+        <v>59</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -1817,6 +1842,12 @@
       <c r="U9" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W9" t="s">
+        <v>59</v>
+      </c>
+      <c r="X9" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -2577,6 +2608,12 @@
       <c r="U19" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W19" t="s">
+        <v>59</v>
+      </c>
+      <c r="X19" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -2950,6 +2987,12 @@
       <c r="U24" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W24" t="s">
+        <v>59</v>
+      </c>
+      <c r="X24" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -3246,6 +3289,12 @@
       <c r="U28" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W28" t="s">
+        <v>59</v>
+      </c>
+      <c r="X28" s="10" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -4081,6 +4130,12 @@
       <c r="U39" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W39" t="s">
+        <v>59</v>
+      </c>
+      <c r="X39" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40">
@@ -4827,6 +4882,12 @@
       <c r="U49" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W49" t="s">
+        <v>59</v>
+      </c>
+      <c r="X49" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50">
@@ -5964,6 +6025,12 @@
       <c r="U64" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W64" t="s">
+        <v>59</v>
+      </c>
+      <c r="X64" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A65">
@@ -6331,6 +6398,12 @@
       <c r="U69" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W69" t="s">
+        <v>59</v>
+      </c>
+      <c r="X69" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A70">
@@ -6867,7 +6940,7 @@
       <c r="W76" t="s">
         <v>59</v>
       </c>
-      <c r="X76" s="9" t="s">
+      <c r="X76" s="4" t="s">
         <v>64</v>
       </c>
     </row>
@@ -7013,6 +7086,12 @@
       <c r="U78" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W78" t="s">
+        <v>59</v>
+      </c>
+      <c r="X78" s="9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79">
@@ -7084,6 +7163,12 @@
       <c r="U79" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W79" t="s">
+        <v>59</v>
+      </c>
+      <c r="X79" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A80">
@@ -7155,8 +7240,14 @@
       <c r="U80" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W80" t="s">
+        <v>59</v>
+      </c>
+      <c r="X80" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81">
         <f t="shared" si="17"/>
         <v>80</v>
@@ -7226,8 +7317,14 @@
       <c r="U81" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W81" t="s">
+        <v>59</v>
+      </c>
+      <c r="X81" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82">
         <f t="shared" si="17"/>
         <v>81</v>
@@ -7297,8 +7394,14 @@
       <c r="U82" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W82" t="s">
+        <v>59</v>
+      </c>
+      <c r="X82" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83">
         <f t="shared" si="17"/>
         <v>82</v>
@@ -7369,7 +7472,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84">
         <f t="shared" si="17"/>
         <v>83</v>
@@ -7439,8 +7542,14 @@
       <c r="U84" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W84" t="s">
+        <v>59</v>
+      </c>
+      <c r="X84" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A85">
         <f t="shared" si="17"/>
         <v>84</v>
@@ -7510,8 +7619,14 @@
       <c r="U85" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W85" t="s">
+        <v>59</v>
+      </c>
+      <c r="X85" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86">
         <f t="shared" si="17"/>
         <v>85</v>
@@ -7581,8 +7696,14 @@
       <c r="U86" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W86" t="s">
+        <v>59</v>
+      </c>
+      <c r="X86" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87">
         <f t="shared" si="17"/>
         <v>86</v>
@@ -7652,8 +7773,14 @@
       <c r="U87" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W87" t="s">
+        <v>59</v>
+      </c>
+      <c r="X87" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88">
         <f t="shared" si="17"/>
         <v>87</v>
@@ -7723,8 +7850,14 @@
       <c r="U88" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W88" t="s">
+        <v>59</v>
+      </c>
+      <c r="X88" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A89">
         <f t="shared" si="17"/>
         <v>88</v>
@@ -7794,8 +7927,14 @@
       <c r="U89" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W89" t="s">
+        <v>59</v>
+      </c>
+      <c r="X89" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90">
         <f t="shared" si="17"/>
         <v>89</v>
@@ -7865,8 +8004,14 @@
       <c r="U90" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W90" t="s">
+        <v>59</v>
+      </c>
+      <c r="X90" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A91">
         <f t="shared" si="17"/>
         <v>90</v>
@@ -7936,8 +8081,14 @@
       <c r="U91" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W91" t="s">
+        <v>59</v>
+      </c>
+      <c r="X91" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92">
         <f t="shared" si="17"/>
         <v>91</v>
@@ -8007,8 +8158,14 @@
       <c r="U92" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W92" t="s">
+        <v>59</v>
+      </c>
+      <c r="X92" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93">
         <f t="shared" si="17"/>
         <v>92</v>
@@ -8078,8 +8235,14 @@
       <c r="U93" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W93" t="s">
+        <v>59</v>
+      </c>
+      <c r="X93" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A94">
         <f t="shared" si="17"/>
         <v>93</v>
@@ -8149,8 +8312,14 @@
       <c r="U94" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W94" t="s">
+        <v>59</v>
+      </c>
+      <c r="X94" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" si="17"/>
         <v>94</v>
@@ -8220,8 +8389,14 @@
       <c r="U95" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W95" t="s">
+        <v>59</v>
+      </c>
+      <c r="X95" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" si="17"/>
         <v>95</v>
@@ -8291,8 +8466,14 @@
       <c r="U96" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W96" t="s">
+        <v>59</v>
+      </c>
+      <c r="X96" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" si="17"/>
         <v>96</v>
@@ -8363,7 +8544,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A98">
         <f t="shared" si="17"/>
         <v>97</v>
@@ -8433,8 +8614,14 @@
       <c r="U98" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W98" t="s">
+        <v>59</v>
+      </c>
+      <c r="X98" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A99">
         <f t="shared" si="17"/>
         <v>98</v>
@@ -8504,8 +8691,14 @@
       <c r="U99" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W99" t="s">
+        <v>59</v>
+      </c>
+      <c r="X99" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A100">
         <f t="shared" si="17"/>
         <v>99</v>
@@ -8575,8 +8768,14 @@
       <c r="U100" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W100" t="s">
+        <v>59</v>
+      </c>
+      <c r="X100" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A101">
         <f t="shared" si="17"/>
         <v>100</v>
@@ -8646,8 +8845,14 @@
       <c r="U101" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W101" t="s">
+        <v>59</v>
+      </c>
+      <c r="X101" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A102">
         <f t="shared" si="17"/>
         <v>101</v>
@@ -8717,8 +8922,14 @@
       <c r="U102" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W102" t="s">
+        <v>59</v>
+      </c>
+      <c r="X102" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A103">
         <f t="shared" si="17"/>
         <v>102</v>
@@ -8788,8 +8999,14 @@
       <c r="U103" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W103" t="s">
+        <v>59</v>
+      </c>
+      <c r="X103" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A104">
         <f t="shared" si="17"/>
         <v>103</v>
@@ -8859,8 +9076,14 @@
       <c r="U104" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W104" t="s">
+        <v>59</v>
+      </c>
+      <c r="X104" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A105">
         <f t="shared" si="17"/>
         <v>104</v>
@@ -8930,8 +9153,14 @@
       <c r="U105" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W105" t="s">
+        <v>59</v>
+      </c>
+      <c r="X105" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A106">
         <f t="shared" si="17"/>
         <v>105</v>
@@ -9001,8 +9230,14 @@
       <c r="U106" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W106" t="s">
+        <v>59</v>
+      </c>
+      <c r="X106" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A107">
         <f t="shared" si="17"/>
         <v>106</v>
@@ -9073,7 +9308,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A108">
         <f t="shared" si="17"/>
         <v>107</v>
@@ -9144,7 +9379,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A109">
         <f t="shared" si="17"/>
         <v>108</v>
@@ -9214,8 +9449,14 @@
       <c r="U109" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W109" t="s">
+        <v>59</v>
+      </c>
+      <c r="X109" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="110" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A110">
         <f t="shared" si="17"/>
         <v>109</v>
@@ -9285,8 +9526,14 @@
       <c r="U110" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W110" t="s">
+        <v>59</v>
+      </c>
+      <c r="X110" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A111">
         <f t="shared" si="17"/>
         <v>110</v>
@@ -9356,8 +9603,14 @@
       <c r="U111" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W111" t="s">
+        <v>59</v>
+      </c>
+      <c r="X111" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="112" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A112">
         <f t="shared" si="17"/>
         <v>111</v>
@@ -9427,8 +9680,14 @@
       <c r="U112" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W112" t="s">
+        <v>59</v>
+      </c>
+      <c r="X112" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A113">
         <f t="shared" si="17"/>
         <v>112</v>
@@ -9498,8 +9757,14 @@
       <c r="U113" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W113" t="s">
+        <v>59</v>
+      </c>
+      <c r="X113" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="114" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A114">
         <f t="shared" si="17"/>
         <v>113</v>
@@ -9569,8 +9834,14 @@
       <c r="U114" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W114" t="s">
+        <v>59</v>
+      </c>
+      <c r="X114" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A115">
         <f t="shared" si="17"/>
         <v>114</v>
@@ -9640,8 +9911,14 @@
       <c r="U115" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W115" t="s">
+        <v>59</v>
+      </c>
+      <c r="X115" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A116">
         <f t="shared" si="17"/>
         <v>115</v>
@@ -9711,8 +9988,14 @@
       <c r="U116" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W116" t="s">
+        <v>59</v>
+      </c>
+      <c r="X116" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A117">
         <f t="shared" si="17"/>
         <v>116</v>
@@ -9782,8 +10065,14 @@
       <c r="U117" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W117" t="s">
+        <v>59</v>
+      </c>
+      <c r="X117" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="118" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A118">
         <f t="shared" si="17"/>
         <v>117</v>
@@ -9853,8 +10142,14 @@
       <c r="U118" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W118" t="s">
+        <v>59</v>
+      </c>
+      <c r="X118" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="119" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A119">
         <f t="shared" si="17"/>
         <v>118</v>
@@ -9924,8 +10219,14 @@
       <c r="U119" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W119" t="s">
+        <v>59</v>
+      </c>
+      <c r="X119" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="120" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A120">
         <f t="shared" si="17"/>
         <v>119</v>
@@ -9995,8 +10296,14 @@
       <c r="U120" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W120" t="s">
+        <v>59</v>
+      </c>
+      <c r="X120" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="121" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A121">
         <f t="shared" si="17"/>
         <v>120</v>
@@ -10066,8 +10373,14 @@
       <c r="U121" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W121" t="s">
+        <v>59</v>
+      </c>
+      <c r="X121" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="122" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A122">
         <f t="shared" si="17"/>
         <v>121</v>
@@ -10137,8 +10450,14 @@
       <c r="U122" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W122" t="s">
+        <v>59</v>
+      </c>
+      <c r="X122" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A123">
         <f t="shared" si="17"/>
         <v>122</v>
@@ -10208,8 +10527,14 @@
       <c r="U123" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W123" t="s">
+        <v>59</v>
+      </c>
+      <c r="X123" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="124" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A124">
         <f t="shared" si="17"/>
         <v>123</v>
@@ -10279,8 +10604,14 @@
       <c r="U124" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W124" t="s">
+        <v>59</v>
+      </c>
+      <c r="X124" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="125" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A125">
         <f t="shared" si="17"/>
         <v>124</v>
@@ -10351,7 +10682,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A126">
         <f t="shared" si="17"/>
         <v>125</v>
@@ -10422,7 +10753,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A127">
         <f t="shared" si="17"/>
         <v>126</v>
@@ -10493,7 +10824,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A128">
         <f t="shared" si="17"/>
         <v>127</v>
@@ -10564,7 +10895,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A129">
         <f t="shared" si="17"/>
         <v>128</v>
@@ -10634,8 +10965,17 @@
       <c r="U129" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W129" t="s">
+        <v>59</v>
+      </c>
+      <c r="X129" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y129" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="130" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" si="17"/>
         <v>129</v>
@@ -10705,8 +11045,14 @@
       <c r="U130" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W130" t="s">
+        <v>59</v>
+      </c>
+      <c r="X130" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="131" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A131">
         <f t="shared" si="17"/>
         <v>130</v>
@@ -10776,8 +11122,14 @@
       <c r="U131" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W131" t="s">
+        <v>59</v>
+      </c>
+      <c r="X131" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="132" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A132">
         <f t="shared" ref="A132:A166" si="26">A131+1</f>
         <v>131</v>
@@ -10847,8 +11199,14 @@
       <c r="U132" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W132" t="s">
+        <v>59</v>
+      </c>
+      <c r="X132" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="133" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A133">
         <f t="shared" si="26"/>
         <v>132</v>
@@ -10918,8 +11276,14 @@
       <c r="U133" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W133" t="s">
+        <v>59</v>
+      </c>
+      <c r="X133" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="134" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A134">
         <f t="shared" si="26"/>
         <v>133</v>
@@ -10989,8 +11353,14 @@
       <c r="U134" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W134" t="s">
+        <v>59</v>
+      </c>
+      <c r="X134" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="135" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A135">
         <f t="shared" si="26"/>
         <v>134</v>
@@ -11060,8 +11430,14 @@
       <c r="U135" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W135" t="s">
+        <v>59</v>
+      </c>
+      <c r="X135" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="136" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A136">
         <f t="shared" si="26"/>
         <v>135</v>
@@ -11131,8 +11507,14 @@
       <c r="U136" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W136" t="s">
+        <v>59</v>
+      </c>
+      <c r="X136" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="137" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A137">
         <f t="shared" si="26"/>
         <v>136</v>
@@ -11202,8 +11584,14 @@
       <c r="U137" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W137" t="s">
+        <v>59</v>
+      </c>
+      <c r="X137" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="138" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A138">
         <f t="shared" si="26"/>
         <v>137</v>
@@ -11274,7 +11662,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A139">
         <f t="shared" si="26"/>
         <v>138</v>
@@ -11345,7 +11733,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A140">
         <f t="shared" si="26"/>
         <v>139</v>
@@ -11416,7 +11804,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A141">
         <f t="shared" si="26"/>
         <v>140</v>
@@ -11486,8 +11874,14 @@
       <c r="U141" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W141" t="s">
+        <v>59</v>
+      </c>
+      <c r="X141" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="142" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A142">
         <f t="shared" si="26"/>
         <v>141</v>
@@ -11558,7 +11952,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A143">
         <f t="shared" si="26"/>
         <v>142</v>
@@ -11629,7 +12023,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A144">
         <f t="shared" si="26"/>
         <v>143</v>
@@ -11700,7 +12094,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="145" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A145">
         <f t="shared" si="26"/>
         <v>144</v>
@@ -11770,8 +12164,14 @@
       <c r="U145" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="146" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W145" t="s">
+        <v>59</v>
+      </c>
+      <c r="X145" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="146" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A146">
         <f t="shared" si="26"/>
         <v>145</v>
@@ -11841,8 +12241,14 @@
       <c r="U146" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="147" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W146" t="s">
+        <v>59</v>
+      </c>
+      <c r="X146" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="147" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A147">
         <f t="shared" si="26"/>
         <v>146</v>
@@ -11912,8 +12318,14 @@
       <c r="U147" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="148" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W147" t="s">
+        <v>59</v>
+      </c>
+      <c r="X147" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="148" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A148">
         <f t="shared" si="26"/>
         <v>147</v>
@@ -11983,8 +12395,14 @@
       <c r="U148" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="149" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W148" t="s">
+        <v>59</v>
+      </c>
+      <c r="X148" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="149" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A149">
         <f t="shared" si="26"/>
         <v>148</v>
@@ -12054,8 +12472,14 @@
       <c r="U149" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="150" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W149" t="s">
+        <v>59</v>
+      </c>
+      <c r="X149" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="150" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A150">
         <f t="shared" si="26"/>
         <v>149</v>
@@ -12125,8 +12549,14 @@
       <c r="U150" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="151" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W150" t="s">
+        <v>59</v>
+      </c>
+      <c r="X150" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="151" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A151">
         <f t="shared" si="26"/>
         <v>150</v>
@@ -12196,8 +12626,14 @@
       <c r="U151" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="152" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W151" t="s">
+        <v>59</v>
+      </c>
+      <c r="X151" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="152" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A152">
         <f t="shared" si="26"/>
         <v>151</v>
@@ -12266,8 +12702,14 @@
       <c r="U152" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="153" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W152" t="s">
+        <v>59</v>
+      </c>
+      <c r="X152" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="153" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A153">
         <f t="shared" si="26"/>
         <v>152</v>
@@ -12336,7 +12778,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="154" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A154">
         <f t="shared" si="26"/>
         <v>153</v>
@@ -12405,7 +12847,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="155" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A155">
         <f t="shared" si="26"/>
         <v>154</v>
@@ -12475,7 +12917,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="156" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A156">
         <f t="shared" si="26"/>
         <v>155</v>
@@ -12544,8 +12986,14 @@
       <c r="U156" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="157" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W156" t="s">
+        <v>59</v>
+      </c>
+      <c r="X156" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="157" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A157">
         <f t="shared" si="26"/>
         <v>156</v>
@@ -12615,7 +13063,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="158" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A158">
         <f t="shared" si="26"/>
         <v>157</v>
@@ -12685,7 +13133,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="159" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A159">
         <f t="shared" si="26"/>
         <v>158</v>
@@ -12755,7 +13203,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="160" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A160">
         <f t="shared" si="26"/>
         <v>159</v>
@@ -12823,6 +13271,12 @@
       </c>
       <c r="U160" s="8" t="s">
         <v>57</v>
+      </c>
+      <c r="W160" t="s">
+        <v>59</v>
+      </c>
+      <c r="X160" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="161" spans="1:24" x14ac:dyDescent="0.2">
@@ -13104,6 +13558,12 @@
       <c r="U164" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W164" t="s">
+        <v>59</v>
+      </c>
+      <c r="X164" s="9" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="165" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A165">
@@ -13174,6 +13634,12 @@
       <c r="U165" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W165" t="s">
+        <v>59</v>
+      </c>
+      <c r="X165" s="9" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="166" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A166">
@@ -13244,11 +13710,17 @@
       <c r="U166" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W166" t="s">
+        <v>59</v>
+      </c>
+      <c r="X166" s="10" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="169" spans="1:24" x14ac:dyDescent="0.2">
       <c r="W169">
         <f>SUBTOTAL(3,W2:W166)</f>
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="X169" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
updates to reporting of rest of runs
</commit_message>
<xml_diff>
--- a/example_project/res_testing_inputs.xlsx
+++ b/example_project/res_testing_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgoldwas/Documents/GitHub/URBANopt/urbanopt-example-geojson-project/example_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AF5F65-9EC3-654A-9978-71AA43784CBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BC4BEF-5968-E74E-9299-47E721533B0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="res_testing_inputs" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="75">
   <si>
     <t>id</t>
   </si>
@@ -254,9 +254,6 @@
   </si>
   <si>
     <t>** Severe  ** Problem found in EMS EnergyPlus Runtime Language</t>
-  </si>
-  <si>
-    <t>I need to check closer for other errors like this that I may have missed skimming through results</t>
   </si>
   <si>
     <t>** Severe  ** Plant temperatures are getting far too hot, check controls and relative loads and capacities</t>
@@ -1152,10 +1149,10 @@
   <dimension ref="A1:Y169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W4" sqref="W4:X4"/>
+      <selection pane="bottomRight" activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1176,6 +1173,7 @@
     <col min="17" max="17" width="21.83203125" style="7" customWidth="1"/>
     <col min="19" max="20" width="10.83203125" style="8"/>
     <col min="21" max="21" width="36.1640625" style="8" customWidth="1"/>
+    <col min="22" max="22" width="10.83203125" customWidth="1"/>
     <col min="23" max="23" width="15.6640625" customWidth="1"/>
     <col min="24" max="24" width="86.1640625" customWidth="1"/>
     <col min="25" max="25" width="61.83203125" customWidth="1"/>
@@ -3293,7 +3291,7 @@
         <v>59</v>
       </c>
       <c r="X28" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
@@ -7777,7 +7775,7 @@
         <v>59</v>
       </c>
       <c r="X87" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.2">
@@ -7854,7 +7852,7 @@
         <v>59</v>
       </c>
       <c r="X88" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.2">
@@ -9003,7 +9001,7 @@
         <v>59</v>
       </c>
       <c r="X103" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.2">
@@ -10069,7 +10067,7 @@
         <v>59</v>
       </c>
       <c r="X117" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="118" spans="1:24" x14ac:dyDescent="0.2">
@@ -10895,7 +10893,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A129">
         <f t="shared" si="17"/>
         <v>128</v>
@@ -10971,11 +10969,8 @@
       <c r="X129" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="Y129" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" si="17"/>
         <v>129</v>
@@ -11052,7 +11047,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A131">
         <f t="shared" si="17"/>
         <v>130</v>
@@ -11129,7 +11124,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A132">
         <f t="shared" ref="A132:A166" si="26">A131+1</f>
         <v>131</v>
@@ -11206,7 +11201,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A133">
         <f t="shared" si="26"/>
         <v>132</v>
@@ -11283,7 +11278,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A134">
         <f t="shared" si="26"/>
         <v>133</v>
@@ -11360,7 +11355,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A135">
         <f t="shared" si="26"/>
         <v>134</v>
@@ -11437,7 +11432,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A136">
         <f t="shared" si="26"/>
         <v>135</v>
@@ -11514,7 +11509,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A137">
         <f t="shared" si="26"/>
         <v>136</v>
@@ -11591,7 +11586,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A138">
         <f t="shared" si="26"/>
         <v>137</v>
@@ -11662,7 +11657,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A139">
         <f t="shared" si="26"/>
         <v>138</v>
@@ -11733,7 +11728,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A140">
         <f t="shared" si="26"/>
         <v>139</v>
@@ -11804,7 +11799,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A141">
         <f t="shared" si="26"/>
         <v>140</v>
@@ -11881,7 +11876,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A142">
         <f t="shared" si="26"/>
         <v>141</v>
@@ -11952,7 +11947,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A143">
         <f t="shared" si="26"/>
         <v>142</v>
@@ -12023,7 +12018,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A144">
         <f t="shared" si="26"/>
         <v>143</v>
@@ -12322,7 +12317,7 @@
         <v>59</v>
       </c>
       <c r="X147" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="148" spans="1:24" x14ac:dyDescent="0.2">
@@ -12399,7 +12394,7 @@
         <v>59</v>
       </c>
       <c r="X148" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="149" spans="1:24" x14ac:dyDescent="0.2">
@@ -13714,7 +13709,7 @@
         <v>59</v>
       </c>
       <c r="X166" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="169" spans="1:24" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
adding log results from todays today
</commit_message>
<xml_diff>
--- a/example_project/res_testing_inputs.xlsx
+++ b/example_project/res_testing_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgoldwas/Documents/GitHub/URBANopt/urbanopt-example-geojson-project/example_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92615C07-44F4-8D40-9EB1-F67C16CAF950}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781CFFE8-4737-8D48-80E4-FC2BA04E78A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2912" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2719" uniqueCount="78">
   <si>
     <t>id</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>Expected 1 element(s) for xpath: AnnualCoolingEfficiency[Units="EER" ](HeatPumpType="ground-to-air)</t>
+  </si>
+  <si>
+    <t>4/1 test results</t>
+  </si>
+  <si>
+    <t>** Severe  ** Invalid EMS Variable Name=EVAP_COOLER_SUPPLY_FAN_CLG</t>
+  </si>
+  <si>
+    <t>undefined method `surfaces' for nil:NilClass&gt; (BuildResidentialHPXML/resources/geometry.rb:1821:in )</t>
   </si>
 </sst>
 </file>
@@ -1151,10 +1160,10 @@
   <dimension ref="A1:Y169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B171" sqref="B171"/>
+      <selection pane="bottomRight" activeCell="M196" sqref="M196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1167,7 +1176,7 @@
     <col min="7" max="8" width="19" style="3" customWidth="1"/>
     <col min="9" max="9" width="29.33203125" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="39.1640625" customWidth="1"/>
+    <col min="11" max="11" width="52.5" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
     <col min="13" max="13" width="19" style="3" customWidth="1"/>
     <col min="14" max="14" width="50.33203125" customWidth="1"/>
@@ -1244,7 +1253,7 @@
         <v>56</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="X1" s="4" t="s">
         <v>60</v>
@@ -1322,12 +1331,8 @@
       <c r="U2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W2" t="s">
-        <v>59</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -1399,6 +1404,8 @@
       <c r="U3" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1470,12 +1477,8 @@
       <c r="U4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W4" t="s">
-        <v>59</v>
-      </c>
-      <c r="X4" s="10" t="s">
-        <v>72</v>
-      </c>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -1547,11 +1550,11 @@
       <c r="U5" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X5" t="s">
-        <v>63</v>
+      <c r="X5" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
@@ -1624,12 +1627,8 @@
       <c r="U6" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W6" t="s">
-        <v>59</v>
-      </c>
-      <c r="X6" t="s">
-        <v>64</v>
-      </c>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -1701,6 +1700,8 @@
       <c r="U7" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1772,6 +1773,8 @@
       <c r="U8" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -1843,11 +1846,11 @@
       <c r="U9" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W9" t="s">
+      <c r="W9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X9" s="10" t="s">
-        <v>72</v>
+      <c r="X9" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
@@ -1920,12 +1923,8 @@
       <c r="U10" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W10" t="s">
-        <v>59</v>
-      </c>
-      <c r="X10" t="s">
-        <v>63</v>
-      </c>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1997,12 +1996,8 @@
       <c r="U11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W11" t="s">
-        <v>59</v>
-      </c>
-      <c r="X11" t="s">
-        <v>64</v>
-      </c>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -2074,12 +2069,8 @@
       <c r="U12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W12" t="s">
-        <v>59</v>
-      </c>
-      <c r="X12" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -2151,11 +2142,11 @@
       <c r="U13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W13" t="s">
+      <c r="W13" s="4" t="s">
         <v>59</v>
       </c>
       <c r="X13" s="9" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
@@ -2228,12 +2219,8 @@
       <c r="U14" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W14" t="s">
-        <v>59</v>
-      </c>
-      <c r="X14" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -2305,12 +2292,8 @@
       <c r="U15" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W15" t="s">
-        <v>59</v>
-      </c>
-      <c r="X15" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -2382,14 +2365,10 @@
       <c r="U16" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W16" t="s">
-        <v>59</v>
-      </c>
-      <c r="X16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="8"/>
         <v>16</v>
@@ -2459,11 +2438,10 @@
       <c r="U17" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="Y17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="8"/>
         <v>17</v>
@@ -2533,14 +2511,10 @@
       <c r="U18" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W18" t="s">
-        <v>59</v>
-      </c>
-      <c r="X18" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -2610,14 +2584,10 @@
       <c r="U19" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W19" t="s">
-        <v>59</v>
-      </c>
-      <c r="X19" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -2687,14 +2657,14 @@
       <c r="U20" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W20" t="s">
+      <c r="W20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="X20" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -2764,14 +2734,10 @@
       <c r="U21" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W21" t="s">
-        <v>59</v>
-      </c>
-      <c r="X21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -2841,14 +2807,10 @@
       <c r="U22" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W22" t="s">
-        <v>59</v>
-      </c>
-      <c r="X22" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -2918,8 +2880,10 @@
       <c r="U23" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -2989,14 +2953,14 @@
       <c r="U24" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W24" t="s">
+      <c r="W24" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X24" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="X24" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -3066,14 +3030,10 @@
       <c r="U25" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W25" t="s">
-        <v>59</v>
-      </c>
-      <c r="X25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="8"/>
         <v>25</v>
@@ -3143,14 +3103,10 @@
       <c r="U26" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W26" t="s">
-        <v>59</v>
-      </c>
-      <c r="X26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="8"/>
         <v>26</v>
@@ -3220,8 +3176,10 @@
       <c r="U27" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="8"/>
         <v>27</v>
@@ -3291,14 +3249,14 @@
       <c r="U28" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W28" t="s">
+      <c r="W28" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X28" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="X28" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="8"/>
         <v>28</v>
@@ -3368,14 +3326,10 @@
       <c r="U29" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W29" t="s">
-        <v>59</v>
-      </c>
-      <c r="X29" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="8"/>
         <v>29</v>
@@ -3445,14 +3399,10 @@
       <c r="U30" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W30" t="s">
-        <v>59</v>
-      </c>
-      <c r="X30" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="8"/>
         <v>30</v>
@@ -3522,14 +3472,10 @@
       <c r="U31" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W31" t="s">
-        <v>59</v>
-      </c>
-      <c r="X31" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="8"/>
         <v>31</v>
@@ -3599,12 +3545,8 @@
       <c r="U32" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W32" t="s">
-        <v>59</v>
-      </c>
-      <c r="X32" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -3676,12 +3618,8 @@
       <c r="U33" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W33" t="s">
-        <v>59</v>
-      </c>
-      <c r="X33" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34">
@@ -3753,12 +3691,8 @@
       <c r="U34" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W34" t="s">
-        <v>59</v>
-      </c>
-      <c r="X34" t="s">
-        <v>69</v>
-      </c>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35">
@@ -3830,11 +3764,11 @@
       <c r="U35" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W35" t="s">
+      <c r="W35" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X35" t="s">
-        <v>63</v>
+      <c r="X35" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
@@ -3907,12 +3841,8 @@
       <c r="U36" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W36" t="s">
-        <v>59</v>
-      </c>
-      <c r="X36" t="s">
-        <v>64</v>
-      </c>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37">
@@ -3984,6 +3914,8 @@
       <c r="U37" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38">
@@ -4055,12 +3987,8 @@
       <c r="U38" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W38" t="s">
-        <v>59</v>
-      </c>
-      <c r="X38" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W38" s="4"/>
+      <c r="X38" s="4"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39">
@@ -4132,11 +4060,11 @@
       <c r="U39" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W39" t="s">
+      <c r="W39" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X39" s="10" t="s">
-        <v>72</v>
+      <c r="X39" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
@@ -4209,12 +4137,8 @@
       <c r="U40" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W40" t="s">
-        <v>59</v>
-      </c>
-      <c r="X40" t="s">
-        <v>63</v>
-      </c>
+      <c r="W40" s="4"/>
+      <c r="X40" s="4"/>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41">
@@ -4286,12 +4210,8 @@
       <c r="U41" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W41" t="s">
-        <v>59</v>
-      </c>
-      <c r="X41" t="s">
-        <v>64</v>
-      </c>
+      <c r="W41" s="4"/>
+      <c r="X41" s="4"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42">
@@ -4363,12 +4283,8 @@
       <c r="U42" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W42" t="s">
-        <v>59</v>
-      </c>
-      <c r="X42" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W42" s="4"/>
+      <c r="X42" s="4"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43">
@@ -4440,6 +4356,12 @@
       <c r="U43" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W43" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="X43" s="9" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44">
@@ -4511,12 +4433,8 @@
       <c r="U44" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W44" t="s">
-        <v>59</v>
-      </c>
-      <c r="X44" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W44" s="4"/>
+      <c r="X44" s="4"/>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45">
@@ -4588,12 +4506,8 @@
       <c r="U45" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W45" t="s">
-        <v>59</v>
-      </c>
-      <c r="X45" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W45" s="4"/>
+      <c r="X45" s="4"/>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46">
@@ -4665,12 +4579,8 @@
       <c r="U46" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W46" t="s">
-        <v>59</v>
-      </c>
-      <c r="X46" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="W46" s="4"/>
+      <c r="X46" s="4"/>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47">
@@ -4742,6 +4652,8 @@
       <c r="U47" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W47" s="4"/>
+      <c r="X47" s="4"/>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48">
@@ -4813,6 +4725,8 @@
       <c r="U48" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W48" s="4"/>
+      <c r="X48" s="4"/>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49">
@@ -4884,12 +4798,8 @@
       <c r="U49" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W49" t="s">
-        <v>59</v>
-      </c>
-      <c r="X49" s="10" t="s">
-        <v>72</v>
-      </c>
+      <c r="W49" s="4"/>
+      <c r="X49" s="4"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50">
@@ -4961,11 +4871,11 @@
       <c r="U50" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W50" t="s">
+      <c r="W50" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X50" t="s">
-        <v>63</v>
+      <c r="X50" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.2">
@@ -5038,12 +4948,8 @@
       <c r="U51" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W51" t="s">
-        <v>59</v>
-      </c>
-      <c r="X51" t="s">
-        <v>64</v>
-      </c>
+      <c r="W51" s="4"/>
+      <c r="X51" s="4"/>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52">
@@ -5115,12 +5021,8 @@
       <c r="U52" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W52" t="s">
-        <v>59</v>
-      </c>
-      <c r="X52" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="W52" s="4"/>
+      <c r="X52" s="4"/>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53">
@@ -5192,12 +5094,8 @@
       <c r="U53" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W53" t="s">
-        <v>59</v>
-      </c>
-      <c r="X53" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="W53" s="4"/>
+      <c r="X53" s="4"/>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54">
@@ -5269,11 +5167,11 @@
       <c r="U54" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W54" t="s">
+      <c r="W54" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X54" t="s">
-        <v>69</v>
+      <c r="X54" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.2">
@@ -5346,12 +5244,8 @@
       <c r="U55" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W55" t="s">
-        <v>59</v>
-      </c>
-      <c r="X55" t="s">
-        <v>63</v>
-      </c>
+      <c r="W55" s="4"/>
+      <c r="X55" s="4"/>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A56">
@@ -5423,12 +5317,8 @@
       <c r="U56" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W56" t="s">
-        <v>59</v>
-      </c>
-      <c r="X56" t="s">
-        <v>64</v>
-      </c>
+      <c r="W56" s="4"/>
+      <c r="X56" s="4"/>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A57">
@@ -5500,6 +5390,8 @@
       <c r="U57" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W57" s="4"/>
+      <c r="X57" s="4"/>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A58">
@@ -5571,11 +5463,11 @@
       <c r="U58" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W58" t="s">
+      <c r="W58" s="4" t="s">
         <v>59</v>
       </c>
       <c r="X58" s="9" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.2">
@@ -5648,12 +5540,8 @@
       <c r="U59" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W59" t="s">
-        <v>59</v>
-      </c>
-      <c r="X59" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W59" s="4"/>
+      <c r="X59" s="4"/>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A60">
@@ -5725,12 +5613,8 @@
       <c r="U60" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W60" t="s">
-        <v>59</v>
-      </c>
-      <c r="X60" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W60" s="4"/>
+      <c r="X60" s="4"/>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A61">
@@ -5802,12 +5686,8 @@
       <c r="U61" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W61" t="s">
-        <v>59</v>
-      </c>
-      <c r="X61" t="s">
-        <v>64</v>
-      </c>
+      <c r="W61" s="4"/>
+      <c r="X61" s="4"/>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62">
@@ -5879,12 +5759,8 @@
       <c r="U62" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W62" t="s">
-        <v>59</v>
-      </c>
-      <c r="X62" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W62" s="4"/>
+      <c r="X62" s="4"/>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63">
@@ -5956,6 +5832,8 @@
       <c r="U63" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W63" s="4"/>
+      <c r="X63" s="4"/>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64">
@@ -6027,12 +5905,8 @@
       <c r="U64" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W64" t="s">
-        <v>59</v>
-      </c>
-      <c r="X64" s="10" t="s">
-        <v>72</v>
-      </c>
+      <c r="W64" s="4"/>
+      <c r="X64" s="4"/>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A65">
@@ -6104,11 +5978,11 @@
       <c r="U65" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W65" t="s">
+      <c r="W65" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X65" t="s">
-        <v>63</v>
+      <c r="X65" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.2">
@@ -6181,12 +6055,8 @@
       <c r="U66" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W66" t="s">
-        <v>59</v>
-      </c>
-      <c r="X66" t="s">
-        <v>64</v>
-      </c>
+      <c r="W66" s="4"/>
+      <c r="X66" s="4"/>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A67">
@@ -6258,6 +6128,8 @@
       <c r="U67" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W67" s="4"/>
+      <c r="X67" s="4"/>
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A68">
@@ -6329,6 +6201,8 @@
       <c r="U68" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W68" s="4"/>
+      <c r="X68" s="4"/>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A69">
@@ -6400,11 +6274,11 @@
       <c r="U69" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W69" t="s">
+      <c r="W69" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X69" s="10" t="s">
-        <v>72</v>
+      <c r="X69" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.2">
@@ -6477,12 +6351,8 @@
       <c r="U70" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W70" t="s">
-        <v>59</v>
-      </c>
-      <c r="X70" t="s">
-        <v>63</v>
-      </c>
+      <c r="W70" s="4"/>
+      <c r="X70" s="4"/>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A71">
@@ -6554,12 +6424,8 @@
       <c r="U71" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W71" t="s">
-        <v>59</v>
-      </c>
-      <c r="X71" t="s">
-        <v>64</v>
-      </c>
+      <c r="W71" s="4"/>
+      <c r="X71" s="4"/>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A72">
@@ -6631,12 +6497,8 @@
       <c r="U72" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W72" t="s">
-        <v>59</v>
-      </c>
-      <c r="X72" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="W72" s="4"/>
+      <c r="X72" s="4"/>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A73">
@@ -6708,11 +6570,11 @@
       <c r="U73" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W73" t="s">
+      <c r="W73" s="4" t="s">
         <v>59</v>
       </c>
       <c r="X73" s="9" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.2">
@@ -6785,12 +6647,8 @@
       <c r="U74" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W74" t="s">
-        <v>59</v>
-      </c>
-      <c r="X74" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W74" s="4"/>
+      <c r="X74" s="4"/>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A75">
@@ -6862,12 +6720,8 @@
       <c r="U75" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W75" t="s">
-        <v>59</v>
-      </c>
-      <c r="X75" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W75" s="4"/>
+      <c r="X75" s="4"/>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A76">
@@ -6939,12 +6793,8 @@
       <c r="U76" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W76" t="s">
-        <v>59</v>
-      </c>
-      <c r="X76" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="W76" s="4"/>
+      <c r="X76" s="4"/>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A77">
@@ -7016,6 +6866,7 @@
       <c r="U77" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W77" s="4"/>
       <c r="X77" s="4"/>
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.2">
@@ -7088,12 +6939,8 @@
       <c r="U78" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W78" t="s">
-        <v>59</v>
-      </c>
-      <c r="X78" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W78" s="4"/>
+      <c r="X78" s="4"/>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79">
@@ -7165,12 +7012,8 @@
       <c r="U79" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W79" t="s">
-        <v>59</v>
-      </c>
-      <c r="X79" s="10" t="s">
-        <v>72</v>
-      </c>
+      <c r="W79" s="4"/>
+      <c r="X79" s="4"/>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A80">
@@ -7242,11 +7085,11 @@
       <c r="U80" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W80" t="s">
+      <c r="W80" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X80" s="4" t="s">
-        <v>63</v>
+      <c r="X80" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.2">
@@ -7319,12 +7162,8 @@
       <c r="U81" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W81" t="s">
-        <v>59</v>
-      </c>
-      <c r="X81" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="W81" s="4"/>
+      <c r="X81" s="4"/>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82">
@@ -7396,12 +7235,8 @@
       <c r="U82" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W82" t="s">
-        <v>59</v>
-      </c>
-      <c r="X82" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W82" s="4"/>
+      <c r="X82" s="4"/>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83">
@@ -7473,6 +7308,8 @@
       <c r="U83" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W83" s="4"/>
+      <c r="X83" s="4"/>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84">
@@ -7544,11 +7381,11 @@
       <c r="U84" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W84" t="s">
+      <c r="W84" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X84" s="10" t="s">
-        <v>72</v>
+      <c r="X84" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.2">
@@ -7621,12 +7458,8 @@
       <c r="U85" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W85" t="s">
-        <v>59</v>
-      </c>
-      <c r="X85" t="s">
-        <v>63</v>
-      </c>
+      <c r="W85" s="4"/>
+      <c r="X85" s="4"/>
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86">
@@ -7698,12 +7531,8 @@
       <c r="U86" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W86" t="s">
-        <v>59</v>
-      </c>
-      <c r="X86" t="s">
-        <v>64</v>
-      </c>
+      <c r="W86" s="4"/>
+      <c r="X86" s="4"/>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87">
@@ -7775,12 +7604,8 @@
       <c r="U87" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W87" t="s">
-        <v>59</v>
-      </c>
-      <c r="X87" s="10" t="s">
-        <v>73</v>
-      </c>
+      <c r="W87" s="4"/>
+      <c r="X87" s="4"/>
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88">
@@ -7852,11 +7677,11 @@
       <c r="U88" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W88" t="s">
+      <c r="W88" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X88" s="10" t="s">
-        <v>73</v>
+      <c r="X88" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.2">
@@ -7929,12 +7754,8 @@
       <c r="U89" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W89" t="s">
-        <v>59</v>
-      </c>
-      <c r="X89" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W89" s="4"/>
+      <c r="X89" s="4"/>
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90">
@@ -8006,12 +7827,8 @@
       <c r="U90" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W90" t="s">
-        <v>59</v>
-      </c>
-      <c r="X90" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W90" s="4"/>
+      <c r="X90" s="4"/>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A91">
@@ -8083,12 +7900,8 @@
       <c r="U91" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W91" t="s">
-        <v>59</v>
-      </c>
-      <c r="X91" t="s">
-        <v>64</v>
-      </c>
+      <c r="W91" s="4"/>
+      <c r="X91" s="4"/>
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92">
@@ -8160,12 +7973,8 @@
       <c r="U92" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W92" t="s">
-        <v>59</v>
-      </c>
-      <c r="X92" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="W92" s="4"/>
+      <c r="X92" s="4"/>
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93">
@@ -8237,12 +8046,8 @@
       <c r="U93" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W93" t="s">
-        <v>59</v>
-      </c>
-      <c r="X93" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="W93" s="4"/>
+      <c r="X93" s="4"/>
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A94">
@@ -8314,12 +8119,8 @@
       <c r="U94" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W94" t="s">
-        <v>59</v>
-      </c>
-      <c r="X94" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="W94" s="4"/>
+      <c r="X94" s="4"/>
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95">
@@ -8391,11 +8192,11 @@
       <c r="U95" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W95" t="s">
+      <c r="W95" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X95" s="4" t="s">
-        <v>63</v>
+      <c r="X95" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.2">
@@ -8468,12 +8269,8 @@
       <c r="U96" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W96" t="s">
-        <v>59</v>
-      </c>
-      <c r="X96" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="W96" s="4"/>
+      <c r="X96" s="4"/>
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A97">
@@ -8545,6 +8342,8 @@
       <c r="U97" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W97" s="4"/>
+      <c r="X97" s="4"/>
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A98">
@@ -8616,12 +8415,8 @@
       <c r="U98" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W98" t="s">
-        <v>59</v>
-      </c>
-      <c r="X98" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W98" s="4"/>
+      <c r="X98" s="4"/>
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A99">
@@ -8693,11 +8488,11 @@
       <c r="U99" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W99" t="s">
+      <c r="W99" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X99" s="10" t="s">
-        <v>72</v>
+      <c r="X99" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.2">
@@ -8770,12 +8565,8 @@
       <c r="U100" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W100" t="s">
-        <v>59</v>
-      </c>
-      <c r="X100" t="s">
-        <v>63</v>
-      </c>
+      <c r="W100" s="4"/>
+      <c r="X100" s="4"/>
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A101">
@@ -8847,12 +8638,8 @@
       <c r="U101" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W101" t="s">
-        <v>59</v>
-      </c>
-      <c r="X101" t="s">
-        <v>64</v>
-      </c>
+      <c r="W101" s="4"/>
+      <c r="X101" s="4"/>
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A102">
@@ -8924,12 +8711,8 @@
       <c r="U102" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W102" t="s">
-        <v>59</v>
-      </c>
-      <c r="X102" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W102" s="4"/>
+      <c r="X102" s="4"/>
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A103">
@@ -9001,11 +8784,11 @@
       <c r="U103" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W103" t="s">
+      <c r="W103" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X103" s="10" t="s">
-        <v>73</v>
+      <c r="X103" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.2">
@@ -9078,12 +8861,8 @@
       <c r="U104" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W104" t="s">
-        <v>59</v>
-      </c>
-      <c r="X104" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W104" s="4"/>
+      <c r="X104" s="4"/>
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A105">
@@ -9155,12 +8934,8 @@
       <c r="U105" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W105" t="s">
-        <v>59</v>
-      </c>
-      <c r="X105" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W105" s="4"/>
+      <c r="X105" s="4"/>
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A106">
@@ -9232,12 +9007,8 @@
       <c r="U106" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W106" t="s">
-        <v>59</v>
-      </c>
-      <c r="X106" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="W106" s="4"/>
+      <c r="X106" s="4"/>
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A107">
@@ -9309,6 +9080,8 @@
       <c r="U107" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W107" s="4"/>
+      <c r="X107" s="4"/>
     </row>
     <row r="108" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A108">
@@ -9380,6 +9153,8 @@
       <c r="U108" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W108" s="4"/>
+      <c r="X108" s="4"/>
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A109">
@@ -9451,12 +9226,8 @@
       <c r="U109" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W109" t="s">
-        <v>59</v>
-      </c>
-      <c r="X109" s="10" t="s">
-        <v>72</v>
-      </c>
+      <c r="W109" s="4"/>
+      <c r="X109" s="4"/>
     </row>
     <row r="110" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A110">
@@ -9528,11 +9299,11 @@
       <c r="U110" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W110" t="s">
+      <c r="W110" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X110" t="s">
-        <v>63</v>
+      <c r="X110" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="111" spans="1:24" x14ac:dyDescent="0.2">
@@ -9605,12 +9376,8 @@
       <c r="U111" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W111" t="s">
-        <v>59</v>
-      </c>
-      <c r="X111" t="s">
-        <v>64</v>
-      </c>
+      <c r="W111" s="4"/>
+      <c r="X111" s="4"/>
     </row>
     <row r="112" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A112">
@@ -9682,12 +9449,8 @@
       <c r="U112" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W112" t="s">
-        <v>59</v>
-      </c>
-      <c r="X112" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="W112" s="4"/>
+      <c r="X112" s="4"/>
     </row>
     <row r="113" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A113">
@@ -9759,12 +9522,8 @@
       <c r="U113" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W113" t="s">
-        <v>59</v>
-      </c>
-      <c r="X113" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="W113" s="4"/>
+      <c r="X113" s="4"/>
     </row>
     <row r="114" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A114">
@@ -9836,11 +9595,11 @@
       <c r="U114" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W114" t="s">
+      <c r="W114" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X114" t="s">
-        <v>69</v>
+      <c r="X114" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="115" spans="1:24" x14ac:dyDescent="0.2">
@@ -9913,12 +9672,8 @@
       <c r="U115" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W115" t="s">
-        <v>59</v>
-      </c>
-      <c r="X115" t="s">
-        <v>63</v>
-      </c>
+      <c r="W115" s="4"/>
+      <c r="X115" s="4"/>
     </row>
     <row r="116" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A116">
@@ -9990,12 +9745,8 @@
       <c r="U116" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W116" t="s">
-        <v>59</v>
-      </c>
-      <c r="X116" t="s">
-        <v>64</v>
-      </c>
+      <c r="W116" s="4"/>
+      <c r="X116" s="4"/>
     </row>
     <row r="117" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A117">
@@ -10067,12 +9818,8 @@
       <c r="U117" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W117" t="s">
-        <v>59</v>
-      </c>
-      <c r="X117" s="10" t="s">
-        <v>73</v>
-      </c>
+      <c r="W117" s="4"/>
+      <c r="X117" s="4"/>
     </row>
     <row r="118" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A118">
@@ -10144,11 +9891,11 @@
       <c r="U118" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W118" t="s">
+      <c r="W118" s="4" t="s">
         <v>59</v>
       </c>
       <c r="X118" s="9" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="119" spans="1:24" x14ac:dyDescent="0.2">
@@ -10221,12 +9968,8 @@
       <c r="U119" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W119" t="s">
-        <v>59</v>
-      </c>
-      <c r="X119" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W119" s="4"/>
+      <c r="X119" s="4"/>
     </row>
     <row r="120" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A120">
@@ -10298,12 +10041,8 @@
       <c r="U120" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W120" t="s">
-        <v>59</v>
-      </c>
-      <c r="X120" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W120" s="4"/>
+      <c r="X120" s="4"/>
     </row>
     <row r="121" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A121">
@@ -10375,12 +10114,8 @@
       <c r="U121" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W121" t="s">
-        <v>59</v>
-      </c>
-      <c r="X121" t="s">
-        <v>64</v>
-      </c>
+      <c r="W121" s="4"/>
+      <c r="X121" s="4"/>
     </row>
     <row r="122" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A122">
@@ -10452,12 +10187,8 @@
       <c r="U122" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W122" t="s">
-        <v>59</v>
-      </c>
-      <c r="X122" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W122" s="4"/>
+      <c r="X122" s="4"/>
     </row>
     <row r="123" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A123">
@@ -10529,12 +10260,8 @@
       <c r="U123" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W123" t="s">
-        <v>59</v>
-      </c>
-      <c r="X123" t="s">
-        <v>63</v>
-      </c>
+      <c r="W123" s="4"/>
+      <c r="X123" s="4"/>
     </row>
     <row r="124" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A124">
@@ -10606,12 +10333,8 @@
       <c r="U124" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W124" t="s">
-        <v>59</v>
-      </c>
-      <c r="X124" s="10" t="s">
-        <v>72</v>
-      </c>
+      <c r="W124" s="4"/>
+      <c r="X124" s="4"/>
     </row>
     <row r="125" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A125">
@@ -10683,6 +10406,12 @@
       <c r="U125" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W125" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="X125" s="9" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="126" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A126">
@@ -10754,6 +10483,8 @@
       <c r="U126" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W126" s="4"/>
+      <c r="X126" s="4"/>
     </row>
     <row r="127" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A127">
@@ -10825,6 +10556,8 @@
       <c r="U127" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W127" s="4"/>
+      <c r="X127" s="4"/>
     </row>
     <row r="128" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A128">
@@ -10896,6 +10629,8 @@
       <c r="U128" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W128" s="4"/>
+      <c r="X128" s="4"/>
     </row>
     <row r="129" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A129">
@@ -10967,11 +10702,11 @@
       <c r="U129" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W129" t="s">
+      <c r="W129" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X129" s="10" t="s">
-        <v>72</v>
+      <c r="X129" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="130" spans="1:24" x14ac:dyDescent="0.2">
@@ -11044,12 +10779,8 @@
       <c r="U130" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W130" t="s">
-        <v>59</v>
-      </c>
-      <c r="X130" t="s">
-        <v>63</v>
-      </c>
+      <c r="W130" s="4"/>
+      <c r="X130" s="4"/>
     </row>
     <row r="131" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A131">
@@ -11121,12 +10852,8 @@
       <c r="U131" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W131" t="s">
-        <v>59</v>
-      </c>
-      <c r="X131" t="s">
-        <v>64</v>
-      </c>
+      <c r="W131" s="4"/>
+      <c r="X131" s="4"/>
     </row>
     <row r="132" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A132">
@@ -11198,12 +10925,8 @@
       <c r="U132" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W132" t="s">
-        <v>59</v>
-      </c>
-      <c r="X132" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="W132" s="4"/>
+      <c r="X132" s="4"/>
     </row>
     <row r="133" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A133">
@@ -11275,11 +10998,11 @@
       <c r="U133" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W133" t="s">
+      <c r="W133" s="4" t="s">
         <v>59</v>
       </c>
       <c r="X133" s="9" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="134" spans="1:24" x14ac:dyDescent="0.2">
@@ -11352,12 +11075,8 @@
       <c r="U134" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W134" t="s">
-        <v>59</v>
-      </c>
-      <c r="X134" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W134" s="4"/>
+      <c r="X134" s="4"/>
     </row>
     <row r="135" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A135">
@@ -11429,12 +11148,8 @@
       <c r="U135" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W135" t="s">
-        <v>59</v>
-      </c>
-      <c r="X135" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W135" s="4"/>
+      <c r="X135" s="4"/>
     </row>
     <row r="136" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A136">
@@ -11506,12 +11221,8 @@
       <c r="U136" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W136" t="s">
-        <v>59</v>
-      </c>
-      <c r="X136" t="s">
-        <v>64</v>
-      </c>
+      <c r="W136" s="4"/>
+      <c r="X136" s="4"/>
     </row>
     <row r="137" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A137">
@@ -11583,12 +11294,8 @@
       <c r="U137" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W137" t="s">
-        <v>59</v>
-      </c>
-      <c r="X137" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W137" s="4"/>
+      <c r="X137" s="4"/>
     </row>
     <row r="138" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A138">
@@ -11660,6 +11367,8 @@
       <c r="U138" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W138" s="4"/>
+      <c r="X138" s="4"/>
     </row>
     <row r="139" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A139">
@@ -11731,6 +11440,8 @@
       <c r="U139" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W139" s="4"/>
+      <c r="X139" s="4"/>
     </row>
     <row r="140" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A140">
@@ -11802,6 +11513,12 @@
       <c r="U140" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W140" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="X140" s="9" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="141" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A141">
@@ -11873,12 +11590,8 @@
       <c r="U141" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W141" t="s">
-        <v>59</v>
-      </c>
-      <c r="X141" t="s">
-        <v>64</v>
-      </c>
+      <c r="W141" s="4"/>
+      <c r="X141" s="4"/>
     </row>
     <row r="142" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A142">
@@ -11950,6 +11663,8 @@
       <c r="U142" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W142" s="4"/>
+      <c r="X142" s="4"/>
     </row>
     <row r="143" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A143">
@@ -12021,6 +11736,8 @@
       <c r="U143" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W143" s="4"/>
+      <c r="X143" s="4"/>
     </row>
     <row r="144" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A144">
@@ -12092,6 +11809,12 @@
       <c r="U144" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W144" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="X144" s="9" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="145" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A145">
@@ -12163,12 +11886,8 @@
       <c r="U145" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W145" t="s">
-        <v>59</v>
-      </c>
-      <c r="X145" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W145" s="4"/>
+      <c r="X145" s="4"/>
     </row>
     <row r="146" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A146">
@@ -12240,12 +11959,8 @@
       <c r="U146" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W146" t="s">
-        <v>59</v>
-      </c>
-      <c r="X146" t="s">
-        <v>64</v>
-      </c>
+      <c r="W146" s="4"/>
+      <c r="X146" s="4"/>
     </row>
     <row r="147" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A147">
@@ -12317,12 +12032,8 @@
       <c r="U147" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W147" t="s">
-        <v>59</v>
-      </c>
-      <c r="X147" s="10" t="s">
-        <v>73</v>
-      </c>
+      <c r="W147" s="4"/>
+      <c r="X147" s="4"/>
     </row>
     <row r="148" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A148">
@@ -12394,11 +12105,11 @@
       <c r="U148" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W148" t="s">
+      <c r="W148" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X148" s="10" t="s">
-        <v>73</v>
+      <c r="X148" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="149" spans="1:24" x14ac:dyDescent="0.2">
@@ -12471,11 +12182,11 @@
       <c r="U149" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W149" t="s">
+      <c r="W149" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X149" s="9" t="s">
-        <v>67</v>
+      <c r="X149" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="150" spans="1:24" x14ac:dyDescent="0.2">
@@ -12548,12 +12259,8 @@
       <c r="U150" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W150" t="s">
-        <v>59</v>
-      </c>
-      <c r="X150" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W150" s="4"/>
+      <c r="X150" s="4"/>
     </row>
     <row r="151" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A151">
@@ -12625,12 +12332,8 @@
       <c r="U151" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W151" t="s">
-        <v>59</v>
-      </c>
-      <c r="X151" t="s">
-        <v>64</v>
-      </c>
+      <c r="W151" s="4"/>
+      <c r="X151" s="4"/>
     </row>
     <row r="152" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A152">
@@ -12701,12 +12404,8 @@
       <c r="U152" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W152" t="s">
-        <v>59</v>
-      </c>
-      <c r="X152" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W152" s="4"/>
+      <c r="X152" s="4"/>
     </row>
     <row r="153" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A153">
@@ -12776,6 +12475,8 @@
       <c r="U153" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W153" s="4"/>
+      <c r="X153" s="4"/>
     </row>
     <row r="154" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A154">
@@ -12845,6 +12546,8 @@
       <c r="U154" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W154" s="4"/>
+      <c r="X154" s="4"/>
     </row>
     <row r="155" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A155">
@@ -12915,6 +12618,8 @@
       <c r="U155" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W155" s="4"/>
+      <c r="X155" s="4"/>
     </row>
     <row r="156" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A156">
@@ -12985,12 +12690,8 @@
       <c r="U156" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W156" t="s">
-        <v>59</v>
-      </c>
-      <c r="X156" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W156" s="4"/>
+      <c r="X156" s="4"/>
     </row>
     <row r="157" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A157">
@@ -13061,6 +12762,8 @@
       <c r="U157" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W157" s="4"/>
+      <c r="X157" s="4"/>
     </row>
     <row r="158" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A158">
@@ -13131,6 +12834,8 @@
       <c r="U158" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W158" s="4"/>
+      <c r="X158" s="4"/>
     </row>
     <row r="159" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A159">
@@ -13201,6 +12906,8 @@
       <c r="U159" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W159" s="4"/>
+      <c r="X159" s="4"/>
     </row>
     <row r="160" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A160">
@@ -13271,12 +12978,8 @@
       <c r="U160" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W160" t="s">
-        <v>59</v>
-      </c>
-      <c r="X160" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="W160" s="4"/>
+      <c r="X160" s="4"/>
     </row>
     <row r="161" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A161">
@@ -13347,6 +13050,8 @@
       <c r="U161" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W161" s="4"/>
+      <c r="X161" s="4"/>
     </row>
     <row r="162" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A162">
@@ -13417,6 +13122,8 @@
       <c r="U162" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W162" s="4"/>
+      <c r="X162" s="4"/>
     </row>
     <row r="163" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A163">
@@ -13487,6 +13194,8 @@
       <c r="U163" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="W163" s="4"/>
+      <c r="X163" s="4"/>
     </row>
     <row r="164" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A164">
@@ -13557,12 +13266,8 @@
       <c r="U164" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W164" t="s">
-        <v>59</v>
-      </c>
-      <c r="X164" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W164" s="4"/>
+      <c r="X164" s="4"/>
     </row>
     <row r="165" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A165">
@@ -13633,12 +13338,8 @@
       <c r="U165" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W165" t="s">
-        <v>59</v>
-      </c>
-      <c r="X165" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="W165" s="4"/>
+      <c r="X165" s="4"/>
     </row>
     <row r="166" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A166">
@@ -13709,17 +13410,13 @@
       <c r="U166" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W166" t="s">
-        <v>59</v>
-      </c>
-      <c r="X166" s="10" t="s">
-        <v>74</v>
-      </c>
+      <c r="W166" s="4"/>
+      <c r="X166" s="4"/>
     </row>
     <row r="169" spans="1:24" x14ac:dyDescent="0.2">
       <c r="W169">
         <f>SUBTOTAL(3,W2:W166)</f>
-        <v>127</v>
+        <v>31</v>
       </c>
       <c r="X169" t="s">
         <v>61</v>
@@ -13931,7 +13628,7 @@
   <dimension ref="A1:Y169"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N138" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="Y17" sqref="Y17"/>

</xml_diff>